<commit_message>
Reduce noise in example Ball-Berry data
</commit_message>
<xml_diff>
--- a/inst/extdata/ball_berry_1.xlsx
+++ b/inst/extdata/ball_berry_1.xlsx
@@ -1911,7 +1911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IF44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BU5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BU11" workbookViewId="0">
       <selection activeCell="CA17" sqref="CA17:CA44"/>
     </sheetView>
   </sheetViews>
@@ -4191,22 +4191,22 @@
       </c>
       <c r="J17">
         <f t="shared" ref="J17:J44" si="0">N17 * AA17 /  BY17</f>
-        <v>8.3399067659873065</v>
+        <v>5.9827786646428871</v>
       </c>
       <c r="K17">
         <v>1629729048.0999999</v>
       </c>
       <c r="L17">
         <f t="shared" ref="L17:L44" si="1">(M17)/1000</f>
-        <v>5.5571256877641247E-3</v>
+        <v>5.3173317687848463E-3</v>
       </c>
       <c r="M17">
         <f t="shared" ref="M17:M44" si="2">1000*CE17*AK17*(CA17-CB17)/(100*BT17*(1000-AK17*CA17))</f>
-        <v>5.5571256877641249</v>
+        <v>5.3173317687848467</v>
       </c>
       <c r="N17">
         <f t="shared" ref="N17:N44" si="3">CE17*AK17*(BZ17-BY17*(1000-AK17*CB17)/(1000-AK17*CA17))/(100*BT17)</f>
-        <v>48.916156033619536</v>
+        <v>35.40047312647134</v>
       </c>
       <c r="O17">
         <f t="shared" ref="O17:O44" si="4">BY17 - IF(AK17&gt;1, N17*BT17*100/(AM17*CM17), 0)</f>
@@ -4214,11 +4214,11 @@
       </c>
       <c r="P17">
         <f t="shared" ref="P17:P44" si="5">((V17-L17/2)*O17-N17)/(V17+L17/2)</f>
-        <v>206.99947517013032</v>
+        <v>252.18043627666717</v>
       </c>
       <c r="Q17">
         <f t="shared" ref="Q17:Q44" si="6">P17*(CF17+CG17)/1000</f>
-        <v>20.54490753900394</v>
+        <v>25.029163683587033</v>
       </c>
       <c r="R17">
         <f t="shared" ref="R17:R44" si="7">(BY17 - IF(AK17&gt;1, N17*BT17*100/(AM17*CM17), 0))*(CF17+CG17)/1000</f>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="S17">
         <f t="shared" ref="S17:S44" si="8">2/((1/U17-1/T17)+SIGN(U17)*SQRT((1/U17-1/T17)*(1/U17-1/T17) + 4*BU17/((BU17+1)*(BU17+1))*(2*1/U17*1/T17-1/T17*1/T17)))</f>
-        <v>0.41573663881322837</v>
+        <v>0.38818854995384178</v>
       </c>
       <c r="T17">
         <f t="shared" ref="T17:T44" si="9">IF(LEFT(BV17,1)&lt;&gt;"0",IF(LEFT(BV17,1)="1",3,BW17),$D$5+$E$5*(CM17*CF17/($K$5*1000))+$F$5*(CM17*CF17/($K$5*1000))*MAX(MIN(BT17,$J$5),$I$5)*MAX(MIN(BT17,$J$5),$I$5)+$G$5*MAX(MIN(BT17,$J$5),$I$5)*(CM17*CF17/($K$5*1000))+$H$5*(CM17*CF17/($K$5*1000))*(CM17*CF17/($K$5*1000)))</f>
@@ -4234,11 +4234,11 @@
       </c>
       <c r="U17">
         <f t="shared" ref="U17:U44" si="10">L17*(1000-(1000*0.61365*EXP(17.502*Y17/(240.97+Y17))/(CF17+CG17)+CA17)/2)/(1000*0.61365*EXP(17.502*Y17/(240.97+Y17))/(CF17+CG17)-CA17)</f>
-        <v>0.385406956919223</v>
+        <v>0.3616074545620791</v>
       </c>
       <c r="V17">
         <f t="shared" ref="V17:V44" si="11">1/((BU17+1)/(S17/1.6)+1/(T17/1.37)) + BU17/((BU17+1)/(S17/1.6) + BU17/(T17/1.37))</f>
-        <v>0.24341970331117796</v>
+        <v>0.22824100921766974</v>
       </c>
       <c r="W17">
         <f t="shared" ref="W17:W44" si="12">(BP17*BS17)</f>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="X17">
         <f t="shared" ref="X17:X44" si="13">(CH17+(W17+2*0.95*0.0000000567*(((CH17+$B$7)+273)^4-(CH17+273)^4)-44100*L17)/(1.84*29.3*T17+8*0.95*0.0000000567*(CH17+273)^3))</f>
-        <v>31.17177732899793</v>
+        <v>31.234218307696715</v>
       </c>
       <c r="Y17">
         <f t="shared" ref="Y17:Y44" si="14">($C$7*CI17+$D$7*CJ17+$E$7*X17)</f>
@@ -4258,11 +4258,11 @@
       </c>
       <c r="AA17">
         <f t="shared" ref="AA17:AA44" si="16">(AB17/AC17*100)</f>
-        <v>70.764179844201905</v>
+        <v>70.145283284868</v>
       </c>
       <c r="AB17">
         <f t="shared" ref="AB17:AB44" si="17">CA17*(CF17+CG17)/1000</f>
-        <v>3.1418976171950277</v>
+        <v>3.1144188895486038</v>
       </c>
       <c r="AC17">
         <f t="shared" ref="AC17:AC44" si="18">0.61365*EXP(17.502*CH17/(240.97+CH17))</f>
@@ -4270,11 +4270,11 @@
       </c>
       <c r="AD17">
         <f t="shared" ref="AD17:AD44" si="19">(Z17-CA17*(CF17+CG17)/1000)</f>
-        <v>1.3758638719467671</v>
+        <v>1.403342599593191</v>
       </c>
       <c r="AE17">
         <f t="shared" ref="AE17:AE44" si="20">(-L17*44100)</f>
-        <v>-245.06924283039791</v>
+        <v>-234.49433100341173</v>
       </c>
       <c r="AF17">
         <f t="shared" ref="AF17:AF44" si="21">2*29.3*T17*0.92*(CH17-Y17)</f>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="AH17">
         <f t="shared" ref="AH17:AH44" si="23">W17+AG17+AE17+AF17</f>
-        <v>24.886334516434552</v>
+        <v>35.461246343420733</v>
       </c>
       <c r="AI17">
         <v>0</v>
@@ -4350,7 +4350,7 @@
       </c>
       <c r="BA17">
         <f t="shared" ref="BA17:BA44" si="30">N17</f>
-        <v>48.916156033619536</v>
+        <v>35.40047312647134</v>
       </c>
       <c r="BB17">
         <f t="shared" ref="BB17:BB44" si="31">AX17*AY17*AZ17</f>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="BC17">
         <f t="shared" ref="BC17:BC44" si="32">(BA17-AS17)/AZ17</f>
-        <v>2.928798092646611E-2</v>
+        <v>2.1248777226177417E-2</v>
       </c>
       <c r="BD17">
         <f t="shared" ref="BD17:BD44" si="33">(AQ17-AW17)/AW17</f>
@@ -4441,10 +4441,10 @@
         <v>415.05399999999997</v>
       </c>
       <c r="BZ17">
-        <v>476.51763104399402</v>
+        <v>460.18032620879899</v>
       </c>
       <c r="CA17">
-        <v>31.656076162082599</v>
+        <v>31.379215232416499</v>
       </c>
       <c r="CB17">
         <v>25.199000000000002</v>
@@ -4960,22 +4960,22 @@
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>1.7769095835232005</v>
+        <v>3.9134054050947795</v>
       </c>
       <c r="K18">
         <v>1629729495.5999999</v>
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
-        <v>4.5120109839883633E-3</v>
+        <v>3.7754599390857711E-3</v>
       </c>
       <c r="M18">
         <f t="shared" si="2"/>
-        <v>4.5120109839883638</v>
+        <v>3.775459939085771</v>
       </c>
       <c r="N18">
         <f t="shared" si="3"/>
-        <v>10.162891134205756</v>
+        <v>22.996635170377214</v>
       </c>
       <c r="O18">
         <f t="shared" si="4"/>
@@ -4983,11 +4983,11 @@
       </c>
       <c r="P18">
         <f t="shared" si="5"/>
-        <v>363.75148424068874</v>
+        <v>280.87970579675704</v>
       </c>
       <c r="Q18">
         <f t="shared" si="6"/>
-        <v>36.105060400759783</v>
+        <v>27.879415431963672</v>
       </c>
       <c r="R18">
         <f t="shared" si="7"/>
@@ -4995,7 +4995,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="8"/>
-        <v>0.3964504578391928</v>
+        <v>0.30448692712343728</v>
       </c>
       <c r="T18">
         <f t="shared" si="9"/>
@@ -5003,11 +5003,11 @@
       </c>
       <c r="U18">
         <f t="shared" si="10"/>
-        <v>0.36868923799374242</v>
+        <v>0.28782087297385078</v>
       </c>
       <c r="V18">
         <f t="shared" si="11"/>
-        <v>0.23276280977466279</v>
+        <v>0.18130936659880226</v>
       </c>
       <c r="W18">
         <f t="shared" si="12"/>
@@ -5015,7 +5015,7 @@
       </c>
       <c r="X18">
         <f t="shared" si="13"/>
-        <v>30.288707717098827</v>
+        <v>30.481098525946749</v>
       </c>
       <c r="Y18">
         <f t="shared" si="14"/>
@@ -5027,11 +5027,11 @@
       </c>
       <c r="AA18">
         <f t="shared" si="16"/>
-        <v>72.552993823444666</v>
+        <v>70.615140357375068</v>
       </c>
       <c r="AB18">
         <f t="shared" si="17"/>
-        <v>3.1653735183036953</v>
+        <v>3.0808280058362612</v>
       </c>
       <c r="AC18">
         <f t="shared" si="18"/>
@@ -5039,11 +5039,11 @@
       </c>
       <c r="AD18">
         <f t="shared" si="19"/>
-        <v>1.1688212915252199</v>
+        <v>1.253366803992654</v>
       </c>
       <c r="AE18">
         <f t="shared" si="20"/>
-        <v>-198.97968439388683</v>
+        <v>-166.4977833136825</v>
       </c>
       <c r="AF18">
         <f t="shared" si="21"/>
@@ -5055,7 +5055,7 @@
       </c>
       <c r="AH18">
         <f t="shared" si="23"/>
-        <v>-1.7553461814918236</v>
+        <v>30.7265548987125</v>
       </c>
       <c r="AI18">
         <v>0</v>
@@ -5119,7 +5119,7 @@
       </c>
       <c r="BA18">
         <f t="shared" si="30"/>
-        <v>10.162891134205756</v>
+        <v>22.996635170377214</v>
       </c>
       <c r="BB18">
         <f t="shared" si="31"/>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="BC18">
         <f t="shared" si="32"/>
-        <v>1.1336391939915204E-2</v>
+        <v>2.5210499832293901E-2</v>
       </c>
       <c r="BD18">
         <f t="shared" si="33"/>
@@ -5210,10 +5210,10 @@
         <v>414.96100000000001</v>
       </c>
       <c r="BZ18">
-        <v>429.40263312036802</v>
+        <v>444.43572662407399</v>
       </c>
       <c r="CA18">
-        <v>31.890524560233398</v>
+        <v>31.038744912046699</v>
       </c>
       <c r="CB18">
         <v>26.649000000000001</v>
@@ -5729,22 +5729,22 @@
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>6.298202104801252</v>
+        <v>4.3390537481030842</v>
       </c>
       <c r="K19">
         <v>1629729851</v>
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
-        <v>4.2950164129533664E-3</v>
+        <v>3.2734835289768426E-3</v>
       </c>
       <c r="M19">
         <f t="shared" si="2"/>
-        <v>4.2950164129533661</v>
+        <v>3.2734835289768425</v>
       </c>
       <c r="N19">
         <f t="shared" si="3"/>
-        <v>35.537820579125587</v>
+        <v>25.430105539382449</v>
       </c>
       <c r="O19">
         <f t="shared" si="4"/>
@@ -5752,11 +5752,11 @@
       </c>
       <c r="P19">
         <f t="shared" si="5"/>
-        <v>264.00101691561849</v>
+        <v>256.75345745044928</v>
       </c>
       <c r="Q19">
         <f t="shared" si="6"/>
-        <v>26.204942451020507</v>
+        <v>25.485544166445671</v>
       </c>
       <c r="R19">
         <f t="shared" si="7"/>
@@ -5764,7 +5764,7 @@
       </c>
       <c r="S19">
         <f t="shared" si="8"/>
-        <v>0.41859242274055297</v>
+        <v>0.28042794895311801</v>
       </c>
       <c r="T19">
         <f t="shared" si="9"/>
@@ -5772,11 +5772,11 @@
       </c>
       <c r="U19">
         <f t="shared" si="10"/>
-        <v>0.3878310622022989</v>
+        <v>0.26625315604387029</v>
       </c>
       <c r="V19">
         <f t="shared" si="11"/>
-        <v>0.24496955112245372</v>
+        <v>0.16762204345213291</v>
       </c>
       <c r="W19">
         <f t="shared" si="12"/>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="X19">
         <f t="shared" si="13"/>
-        <v>29.748083184209531</v>
+        <v>30.014463250828758</v>
       </c>
       <c r="Y19">
         <f t="shared" si="14"/>
@@ -5796,11 +5796,11 @@
       </c>
       <c r="AA19">
         <f t="shared" si="16"/>
-        <v>73.552766819876567</v>
+        <v>70.814155291801669</v>
       </c>
       <c r="AB19">
         <f t="shared" si="17"/>
-        <v>3.1516329466007735</v>
+        <v>3.0342872818080648</v>
       </c>
       <c r="AC19">
         <f t="shared" si="18"/>
@@ -5808,11 +5808,11 @@
       </c>
       <c r="AD19">
         <f t="shared" si="19"/>
-        <v>1.0584948087527937</v>
+        <v>1.1758404735455024</v>
       </c>
       <c r="AE19">
         <f t="shared" si="20"/>
-        <v>-189.41022381124347</v>
+        <v>-144.36062362787877</v>
       </c>
       <c r="AF19">
         <f t="shared" si="21"/>
@@ -5824,7 +5824,7 @@
       </c>
       <c r="AH19">
         <f t="shared" si="23"/>
-        <v>-7.6525304623572197</v>
+        <v>37.397069721007483</v>
       </c>
       <c r="AI19">
         <v>0</v>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="BA19">
         <f t="shared" si="30"/>
-        <v>35.537820579125587</v>
+        <v>25.430105539382449</v>
       </c>
       <c r="BB19">
         <f t="shared" si="31"/>
@@ -5896,7 +5896,7 @@
       </c>
       <c r="BC19">
         <f t="shared" si="32"/>
-        <v>5.3271531106798546E-2</v>
+        <v>3.8256620982710945E-2</v>
       </c>
       <c r="BD19">
         <f t="shared" si="33"/>
@@ -5979,10 +5979,10 @@
         <v>415.024</v>
       </c>
       <c r="BZ19">
-        <v>459.805470987989</v>
+        <v>447.16829419759802</v>
       </c>
       <c r="CA19">
-        <v>31.751044842114101</v>
+        <v>30.568848968422799</v>
       </c>
       <c r="CB19">
         <v>26.760999999999999</v>
@@ -6498,22 +6498,22 @@
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>5.8867236749827603</v>
+        <v>3.9200412389015171</v>
       </c>
       <c r="K20">
         <v>1629730274</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>2.4044917182627001E-3</v>
+        <v>2.6265823042909558E-3</v>
       </c>
       <c r="M20">
         <f t="shared" si="2"/>
-        <v>2.4044917182627001</v>
+        <v>2.626582304290956</v>
       </c>
       <c r="N20">
         <f t="shared" si="3"/>
-        <v>35.279629851904744</v>
+        <v>23.290614005322738</v>
       </c>
       <c r="O20">
         <f t="shared" si="4"/>
@@ -6521,11 +6521,11 @@
       </c>
       <c r="P20">
         <f t="shared" si="5"/>
-        <v>110.56071161374169</v>
+        <v>231.66867028991334</v>
       </c>
       <c r="Q20">
         <f t="shared" si="6"/>
-        <v>10.974556517672744</v>
+        <v>22.996061425085305</v>
       </c>
       <c r="R20">
         <f t="shared" si="7"/>
@@ -6533,7 +6533,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="8"/>
-        <v>0.19468709841142634</v>
+        <v>0.21810229874987541</v>
       </c>
       <c r="T20">
         <f t="shared" si="9"/>
@@ -6541,11 +6541,11 @@
       </c>
       <c r="U20">
         <f t="shared" si="10"/>
-        <v>0.18774425417289542</v>
+        <v>0.2094289954189473</v>
       </c>
       <c r="V20">
         <f t="shared" si="11"/>
-        <v>0.11794331837539387</v>
+        <v>0.13164364438807874</v>
       </c>
       <c r="W20">
         <f t="shared" si="12"/>
@@ -6553,7 +6553,7 @@
       </c>
       <c r="X20">
         <f t="shared" si="13"/>
-        <v>29.950962888910762</v>
+        <v>29.893080380934904</v>
       </c>
       <c r="Y20">
         <f t="shared" si="14"/>
@@ -6565,11 +6565,11 @@
       </c>
       <c r="AA20">
         <f t="shared" si="16"/>
-        <v>69.25349210772076</v>
+        <v>69.85568330248141</v>
       </c>
       <c r="AB20">
         <f t="shared" si="17"/>
-        <v>2.9421992489314026</v>
+        <v>2.9677830343408367</v>
       </c>
       <c r="AC20">
         <f t="shared" si="18"/>
@@ -6577,11 +6577,11 @@
       </c>
       <c r="AD20">
         <f t="shared" si="19"/>
-        <v>1.2257537704454502</v>
+        <v>1.2001699850360161</v>
       </c>
       <c r="AE20">
         <f t="shared" si="20"/>
-        <v>-106.03808477538507</v>
+        <v>-115.83227961923116</v>
       </c>
       <c r="AF20">
         <f t="shared" si="21"/>
@@ -6593,7 +6593,7 @@
       </c>
       <c r="AH20">
         <f t="shared" si="23"/>
-        <v>56.265813130943449</v>
+        <v>46.471618287097364</v>
       </c>
       <c r="AI20">
         <v>0</v>
@@ -6657,7 +6657,7 @@
       </c>
       <c r="BA20">
         <f t="shared" si="30"/>
-        <v>35.279629851904744</v>
+        <v>23.290614005322738</v>
       </c>
       <c r="BB20">
         <f t="shared" si="31"/>
@@ -6665,7 +6665,7 @@
       </c>
       <c r="BC20">
         <f t="shared" si="32"/>
-        <v>6.5068932351285219E-2</v>
+        <v>4.3157544348852821E-2</v>
       </c>
       <c r="BD20">
         <f t="shared" si="33"/>
@@ -6748,10 +6748,10 @@
         <v>415.04199999999997</v>
       </c>
       <c r="BZ20">
-        <v>458.56519059690697</v>
+        <v>444.29223811938101</v>
       </c>
       <c r="CA20">
-        <v>29.6405273550182</v>
+        <v>29.898265471003601</v>
       </c>
       <c r="CB20">
         <v>26.8413</v>
@@ -7267,22 +7267,22 @@
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>2.3879438442369905</v>
+        <v>2.7980680752069333</v>
       </c>
       <c r="K21">
         <v>1629730534</v>
       </c>
       <c r="L21">
         <f t="shared" si="1"/>
-        <v>2.7756040647255449E-3</v>
+        <v>2.5534129886051601E-3</v>
       </c>
       <c r="M21">
         <f t="shared" si="2"/>
-        <v>2.7756040647255449</v>
+        <v>2.5534129886051602</v>
       </c>
       <c r="N21">
         <f t="shared" si="3"/>
-        <v>14.061104122048272</v>
+        <v>16.617928559239719</v>
       </c>
       <c r="O21">
         <f t="shared" si="4"/>
@@ -7290,11 +7290,11 @@
       </c>
       <c r="P21">
         <f t="shared" si="5"/>
-        <v>309.37255325269433</v>
+        <v>278.61693013974303</v>
       </c>
       <c r="Q21">
         <f t="shared" si="6"/>
-        <v>30.702425717475911</v>
+        <v>27.650208498811416</v>
       </c>
       <c r="R21">
         <f t="shared" si="7"/>
@@ -7302,7 +7302,7 @@
       </c>
       <c r="S21">
         <f t="shared" si="8"/>
-        <v>0.23692635120349606</v>
+        <v>0.21238014168663091</v>
       </c>
       <c r="T21">
         <f t="shared" si="9"/>
@@ -7310,11 +7310,11 @@
       </c>
       <c r="U21">
         <f t="shared" si="10"/>
-        <v>0.22672105294469549</v>
+        <v>0.20414035880800271</v>
       </c>
       <c r="V21">
         <f t="shared" si="11"/>
-        <v>0.14258093114989923</v>
+        <v>0.12830139972154195</v>
       </c>
       <c r="W21">
         <f t="shared" si="12"/>
@@ -7322,7 +7322,7 @@
       </c>
       <c r="X21">
         <f t="shared" si="13"/>
-        <v>29.725115524560916</v>
+        <v>29.783067212433444</v>
       </c>
       <c r="Y21">
         <f t="shared" si="14"/>
@@ -7334,11 +7334,11 @@
       </c>
       <c r="AA21">
         <f t="shared" si="16"/>
-        <v>70.485004619639824</v>
+        <v>69.883305005805553</v>
       </c>
       <c r="AB21">
         <f t="shared" si="17"/>
-        <v>2.9966709160998377</v>
+        <v>2.9710896489532193</v>
       </c>
       <c r="AC21">
         <f t="shared" si="18"/>
@@ -7346,11 +7346,11 @@
       </c>
       <c r="AD21">
         <f t="shared" si="19"/>
-        <v>1.1710900435145106</v>
+        <v>1.1966713106611291</v>
       </c>
       <c r="AE21">
         <f t="shared" si="20"/>
-        <v>-122.40413925439653</v>
+        <v>-112.60551279748756</v>
       </c>
       <c r="AF21">
         <f t="shared" si="21"/>
@@ -7362,7 +7362,7 @@
       </c>
       <c r="AH21">
         <f t="shared" si="23"/>
-        <v>18.171923545953753</v>
+        <v>27.970550002862716</v>
       </c>
       <c r="AI21">
         <v>0</v>
@@ -7426,7 +7426,7 @@
       </c>
       <c r="BA21">
         <f t="shared" si="30"/>
-        <v>14.061104122048272</v>
+        <v>16.617928559239719</v>
       </c>
       <c r="BB21">
         <f t="shared" si="31"/>
@@ -7434,7 +7434,7 @@
       </c>
       <c r="BC21">
         <f t="shared" si="32"/>
-        <v>3.414309721146834E-2</v>
+        <v>4.0211969783454399E-2</v>
       </c>
       <c r="BD21">
         <f t="shared" si="33"/>
@@ -7517,10 +7517,10 @@
         <v>415.04199999999997</v>
       </c>
       <c r="BZ21">
-        <v>433.296364838138</v>
+        <v>436.25367296762801</v>
       </c>
       <c r="CA21">
-        <v>30.195911590275301</v>
+        <v>29.9381423180551</v>
       </c>
       <c r="CB21">
         <v>26.966000000000001</v>
@@ -8036,22 +8036,22 @@
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>1.8565007981170947</v>
+        <v>2.0823199989489902</v>
       </c>
       <c r="K22">
         <v>1629730901.5</v>
       </c>
       <c r="L22">
         <f t="shared" si="1"/>
-        <v>2.6950492963641027E-3</v>
+        <v>2.1638602838054636E-3</v>
       </c>
       <c r="M22">
         <f t="shared" si="2"/>
-        <v>2.6950492963641026</v>
+        <v>2.1638602838054637</v>
       </c>
       <c r="N22">
         <f t="shared" si="3"/>
-        <v>10.69358459242148</v>
+        <v>12.240074212238875</v>
       </c>
       <c r="O22">
         <f t="shared" si="4"/>
@@ -8059,11 +8059,11 @@
       </c>
       <c r="P22">
         <f t="shared" si="5"/>
-        <v>335.76467796263671</v>
+        <v>299.02705028291035</v>
       </c>
       <c r="Q22">
         <f t="shared" si="6"/>
-        <v>33.322051613677878</v>
+        <v>29.676125743404686</v>
       </c>
       <c r="R22">
         <f t="shared" si="7"/>
@@ -8071,7 +8071,7 @@
       </c>
       <c r="S22">
         <f t="shared" si="8"/>
-        <v>0.24569022635047222</v>
+        <v>0.18486556916497213</v>
       </c>
       <c r="T22">
         <f t="shared" si="9"/>
@@ -8079,11 +8079,11 @@
       </c>
       <c r="U22">
         <f t="shared" si="10"/>
-        <v>0.23476061175411944</v>
+        <v>0.17860352944166397</v>
       </c>
       <c r="V22">
         <f t="shared" si="11"/>
-        <v>0.1476668443133774</v>
+        <v>0.11217215440676276</v>
       </c>
       <c r="W22">
         <f t="shared" si="12"/>
@@ -8091,7 +8091,7 @@
       </c>
       <c r="X22">
         <f t="shared" si="13"/>
-        <v>29.502673502784354</v>
+        <v>29.640908257613145</v>
       </c>
       <c r="Y22">
         <f t="shared" si="14"/>
@@ -8103,11 +8103,11 @@
       </c>
       <c r="AA22">
         <f t="shared" si="16"/>
-        <v>72.053396977005292</v>
+        <v>70.606721915104856</v>
       </c>
       <c r="AB22">
         <f t="shared" si="17"/>
-        <v>3.0456371407901792</v>
+        <v>2.9844873895774082</v>
       </c>
       <c r="AC22">
         <f t="shared" si="18"/>
@@ -8115,11 +8115,11 @@
       </c>
       <c r="AD22">
         <f t="shared" si="19"/>
-        <v>1.0980336976908665</v>
+        <v>1.1591834489036374</v>
       </c>
       <c r="AE22">
         <f t="shared" si="20"/>
-        <v>-118.85167396965693</v>
+        <v>-95.426238515820941</v>
       </c>
       <c r="AF22">
         <f t="shared" si="21"/>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="AH22">
         <f t="shared" si="23"/>
-        <v>-2.4348582808545487</v>
+        <v>20.990577172981439</v>
       </c>
       <c r="AI22">
         <v>0</v>
@@ -8195,7 +8195,7 @@
       </c>
       <c r="BA22">
         <f t="shared" si="30"/>
-        <v>10.69358459242148</v>
+        <v>12.240074212238875</v>
       </c>
       <c r="BB22">
         <f t="shared" si="31"/>
@@ -8203,7 +8203,7 @@
       </c>
       <c r="BC22">
         <f t="shared" si="32"/>
-        <v>3.7330079807919275E-2</v>
+        <v>4.2570209048559189E-2</v>
       </c>
       <c r="BD22">
         <f t="shared" si="33"/>
@@ -8286,10 +8286,10 @@
         <v>415.03300000000002</v>
       </c>
       <c r="BZ22">
-        <v>429.20527522041198</v>
+        <v>430.79625504408199</v>
       </c>
       <c r="CA22">
-        <v>30.688907922725299</v>
+        <v>30.072741584545099</v>
       </c>
       <c r="CB22">
         <v>27.554600000000001</v>
@@ -8805,22 +8805,22 @@
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>-0.11180287752708432</v>
+        <v>0.96902955315742012</v>
       </c>
       <c r="K23">
         <v>1629731320.5</v>
       </c>
       <c r="L23">
         <f t="shared" si="1"/>
-        <v>2.8725222614000199E-3</v>
+        <v>1.9208197028560226E-3</v>
       </c>
       <c r="M23">
         <f t="shared" si="2"/>
-        <v>2.8725222614000199</v>
+        <v>1.9208197028560225</v>
       </c>
       <c r="N23">
         <f t="shared" si="3"/>
-        <v>-0.63185443553585263</v>
+        <v>5.6791743036248699</v>
       </c>
       <c r="O23">
         <f t="shared" si="4"/>
@@ -8828,11 +8828,11 @@
       </c>
       <c r="P23">
         <f t="shared" si="5"/>
-        <v>411.74060401120499</v>
+        <v>352.43549904851579</v>
       </c>
       <c r="Q23">
         <f t="shared" si="6"/>
-        <v>40.863020843594725</v>
+        <v>34.977310965547353</v>
       </c>
       <c r="R23">
         <f t="shared" si="7"/>
@@ -8840,7 +8840,7 @@
       </c>
       <c r="S23">
         <f t="shared" si="8"/>
-        <v>0.28511669526867517</v>
+        <v>0.1685879563711753</v>
       </c>
       <c r="T23">
         <f t="shared" si="9"/>
@@ -8848,11 +8848,11 @@
       </c>
       <c r="U23">
         <f t="shared" si="10"/>
-        <v>0.27046385911766835</v>
+        <v>0.16334651920023785</v>
       </c>
       <c r="V23">
         <f t="shared" si="11"/>
-        <v>0.17029363384102145</v>
+        <v>0.1025489223782716</v>
       </c>
       <c r="W23">
         <f t="shared" si="12"/>
@@ -8860,7 +8860,7 @@
       </c>
       <c r="X23">
         <f t="shared" si="13"/>
-        <v>29.114532152055077</v>
+        <v>29.36300083308987</v>
       </c>
       <c r="Y23">
         <f t="shared" si="14"/>
@@ -8872,11 +8872,11 @@
       </c>
       <c r="AA23">
         <f t="shared" si="16"/>
-        <v>73.432308096442611</v>
+        <v>70.811380343143682</v>
       </c>
       <c r="AB23">
         <f t="shared" si="17"/>
-        <v>3.0695029939927827</v>
+        <v>2.9599470533675203</v>
       </c>
       <c r="AC23">
         <f t="shared" si="18"/>
@@ -8884,11 +8884,11 @@
       </c>
       <c r="AD23">
         <f t="shared" si="19"/>
-        <v>1.0160533662292166</v>
+        <v>1.125609306854479</v>
       </c>
       <c r="AE23">
         <f t="shared" si="20"/>
-        <v>-126.67823172774088</v>
+        <v>-84.7081488959506</v>
       </c>
       <c r="AF23">
         <f t="shared" si="21"/>
@@ -8900,7 +8900,7 @@
       </c>
       <c r="AH23">
         <f t="shared" si="23"/>
-        <v>-26.641762734912412</v>
+        <v>15.328320096877867</v>
       </c>
       <c r="AI23">
         <v>0</v>
@@ -8964,7 +8964,7 @@
       </c>
       <c r="BA23">
         <f t="shared" si="30"/>
-        <v>-0.63185443553585263</v>
+        <v>5.6791743036248699</v>
       </c>
       <c r="BB23">
         <f t="shared" si="31"/>
@@ -8972,7 +8972,7 @@
       </c>
       <c r="BC23">
         <f t="shared" si="32"/>
-        <v>-1.8282073030462217E-3</v>
+        <v>3.5580869036531806E-2</v>
       </c>
       <c r="BD23">
         <f t="shared" si="33"/>
@@ -9055,10 +9055,10 @@
         <v>415.00299999999999</v>
       </c>
       <c r="BZ23">
-        <v>415.675131727419</v>
+        <v>422.77262634548401</v>
       </c>
       <c r="CA23">
-        <v>30.928673178573799</v>
+        <v>29.8247746357148</v>
       </c>
       <c r="CB23">
         <v>27.589099999999998</v>
@@ -9574,22 +9574,22 @@
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>8.9977202621442363</v>
+        <v>8.2809960737159809</v>
       </c>
       <c r="K24">
         <v>1629733760</v>
       </c>
       <c r="L24">
         <f t="shared" si="1"/>
-        <v>9.2952865743293825E-3</v>
+        <v>8.8466704988126796E-3</v>
       </c>
       <c r="M24">
         <f t="shared" si="2"/>
-        <v>9.2952865743293831</v>
+        <v>8.8466704988126796</v>
       </c>
       <c r="N24">
         <f t="shared" si="3"/>
-        <v>49.088557410846285</v>
+        <v>45.780745924715674</v>
       </c>
       <c r="O24">
         <f t="shared" si="4"/>
@@ -9597,11 +9597,11 @@
       </c>
       <c r="P24">
         <f t="shared" si="5"/>
-        <v>315.94114503669135</v>
+        <v>313.0081040042312</v>
       </c>
       <c r="Q24">
         <f t="shared" si="6"/>
-        <v>31.360274646028657</v>
+        <v>31.069141396146499</v>
       </c>
       <c r="R24">
         <f t="shared" si="7"/>
@@ -9609,7 +9609,7 @@
       </c>
       <c r="S24">
         <f t="shared" si="8"/>
-        <v>0.98146377023380149</v>
+        <v>0.87716797856944773</v>
       </c>
       <c r="T24">
         <f t="shared" si="9"/>
@@ -9617,11 +9617,11 @@
       </c>
       <c r="U24">
         <f t="shared" si="10"/>
-        <v>0.82873539284180431</v>
+        <v>0.75299178083728657</v>
       </c>
       <c r="V24">
         <f t="shared" si="11"/>
-        <v>0.52969000003056799</v>
+        <v>0.48030452616065611</v>
       </c>
       <c r="W24">
         <f t="shared" si="12"/>
@@ -9629,7 +9629,7 @@
       </c>
       <c r="X24">
         <f t="shared" si="13"/>
-        <v>32.563672189113987</v>
+        <v>32.680190668755891</v>
       </c>
       <c r="Y24">
         <f t="shared" si="14"/>
@@ -9641,11 +9641,11 @@
       </c>
       <c r="AA24">
         <f t="shared" si="16"/>
-        <v>76.073020672071138</v>
+        <v>75.072029737785769</v>
       </c>
       <c r="AB24">
         <f t="shared" si="17"/>
-        <v>3.861553991935017</v>
+        <v>3.8107425412520874</v>
       </c>
       <c r="AC24">
         <f t="shared" si="18"/>
@@ -9653,11 +9653,11 @@
       </c>
       <c r="AD24">
         <f t="shared" si="19"/>
-        <v>1.0640420776228159</v>
+        <v>1.1148535283057455</v>
       </c>
       <c r="AE24">
         <f t="shared" si="20"/>
-        <v>-409.92213792792575</v>
+        <v>-390.13816899763918</v>
       </c>
       <c r="AF24">
         <f t="shared" si="21"/>
@@ -9669,7 +9669,7 @@
       </c>
       <c r="AH24">
         <f t="shared" si="23"/>
-        <v>2.4059983035672872</v>
+        <v>22.189967233853849</v>
       </c>
       <c r="AI24">
         <v>0</v>
@@ -9733,7 +9733,7 @@
       </c>
       <c r="BA24">
         <f t="shared" si="30"/>
-        <v>49.088557410846285</v>
+        <v>45.780745924715674</v>
       </c>
       <c r="BB24">
         <f t="shared" si="31"/>
@@ -9741,7 +9741,7 @@
       </c>
       <c r="BC24">
         <f t="shared" si="32"/>
-        <v>2.9391255231636767E-2</v>
+        <v>2.7423701678164061E-2</v>
       </c>
       <c r="BD24">
         <f t="shared" si="33"/>
@@ -9824,10 +9824,10 @@
         <v>415.029</v>
       </c>
       <c r="BZ24">
-        <v>478.55740284507999</v>
+        <v>474.36508056901602</v>
       </c>
       <c r="CA24">
-        <v>38.903479118205198</v>
+        <v>38.391575823640999</v>
       </c>
       <c r="CB24">
         <v>28.1843</v>
@@ -10343,22 +10343,22 @@
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>6.7914582941454205</v>
+        <v>6.5579026370221554</v>
       </c>
       <c r="K25">
         <v>1629734524.5</v>
       </c>
       <c r="L25">
         <f t="shared" si="1"/>
-        <v>6.5051545324349936E-3</v>
+        <v>6.3989563275796682E-3</v>
       </c>
       <c r="M25">
         <f t="shared" si="2"/>
-        <v>6.505154532434994</v>
+        <v>6.3989563275796684</v>
       </c>
       <c r="N25">
         <f t="shared" si="3"/>
-        <v>37.385835088123301</v>
+        <v>36.218245496621854</v>
       </c>
       <c r="O25">
         <f t="shared" si="4"/>
@@ -10366,11 +10366,11 @@
       </c>
       <c r="P25">
         <f t="shared" si="5"/>
-        <v>312.72045811899875</v>
+        <v>312.93101597395247</v>
       </c>
       <c r="Q25">
         <f t="shared" si="6"/>
-        <v>31.042428845387114</v>
+        <v>31.06333002745097</v>
       </c>
       <c r="R25">
         <f t="shared" si="7"/>
@@ -10378,7 +10378,7 @@
       </c>
       <c r="S25">
         <f t="shared" si="8"/>
-        <v>0.69119130298622644</v>
+        <v>0.66951186640511939</v>
       </c>
       <c r="T25">
         <f t="shared" si="9"/>
@@ -10386,11 +10386,11 @@
       </c>
       <c r="U25">
         <f t="shared" si="10"/>
-        <v>0.61153158451858669</v>
+        <v>0.59448150597381821</v>
       </c>
       <c r="V25">
         <f t="shared" si="11"/>
-        <v>0.3885965838259266</v>
+        <v>0.37758905756455824</v>
       </c>
       <c r="W25">
         <f t="shared" si="12"/>
@@ -10398,7 +10398,7 @@
       </c>
       <c r="X25">
         <f t="shared" si="13"/>
-        <v>31.87184705540308</v>
+        <v>31.899444809321103</v>
       </c>
       <c r="Y25">
         <f t="shared" si="14"/>
@@ -10410,11 +10410,11 @@
       </c>
       <c r="AA25">
         <f t="shared" si="16"/>
-        <v>75.391768650724714</v>
+        <v>75.14594252689993</v>
       </c>
       <c r="AB25">
         <f t="shared" si="17"/>
-        <v>3.7061732986102225</v>
+        <v>3.6940887669362001</v>
       </c>
       <c r="AC25">
         <f t="shared" si="18"/>
@@ -10422,11 +10422,11 @@
       </c>
       <c r="AD25">
         <f t="shared" si="19"/>
-        <v>1.0111349822504598</v>
+        <v>1.0232195139244822</v>
       </c>
       <c r="AE25">
         <f t="shared" si="20"/>
-        <v>-286.87731488038321</v>
+        <v>-282.19397404626335</v>
       </c>
       <c r="AF25">
         <f t="shared" si="21"/>
@@ -10438,7 +10438,7 @@
       </c>
       <c r="AH25">
         <f t="shared" si="23"/>
-        <v>14.688943051670421</v>
+        <v>19.372283885790281</v>
       </c>
       <c r="AI25">
         <v>0</v>
@@ -10502,7 +10502,7 @@
       </c>
       <c r="BA25">
         <f t="shared" si="30"/>
-        <v>37.385835088123301</v>
+        <v>36.218245496621854</v>
       </c>
       <c r="BB25">
         <f t="shared" si="31"/>
@@ -10510,7 +10510,7 @@
       </c>
       <c r="BC25">
         <f t="shared" si="32"/>
-        <v>4.0760207503464763E-2</v>
+        <v>3.9498151778749858E-2</v>
       </c>
       <c r="BD25">
         <f t="shared" si="33"/>
@@ -10593,10 +10593,10 @@
         <v>415.01900000000001</v>
       </c>
       <c r="BZ25">
-        <v>463.11940856081299</v>
+        <v>461.665481712163</v>
       </c>
       <c r="CA25">
-        <v>37.335873993056303</v>
+        <v>37.214134798611298</v>
       </c>
       <c r="CB25">
         <v>29.8215</v>
@@ -11112,22 +11112,22 @@
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>7.9881386013595881</v>
+        <v>5.8845276305144569</v>
       </c>
       <c r="K26">
         <v>1629735345.0999999</v>
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
-        <v>5.1845474904762424E-3</v>
+        <v>5.6097827461911833E-3</v>
       </c>
       <c r="M26">
         <f t="shared" si="2"/>
-        <v>5.1845474904762421</v>
+        <v>5.6097827461911836</v>
       </c>
       <c r="N26">
         <f t="shared" si="3"/>
-        <v>45.079934607965569</v>
+        <v>32.769395582938948</v>
       </c>
       <c r="O26">
         <f t="shared" si="4"/>
@@ -11135,11 +11135,11 @@
       </c>
       <c r="P26">
         <f t="shared" si="5"/>
-        <v>249.6532038459882</v>
+        <v>306.53583712486238</v>
       </c>
       <c r="Q26">
         <f t="shared" si="6"/>
-        <v>24.787378815291571</v>
+        <v>30.43509876189631</v>
       </c>
       <c r="R26">
         <f t="shared" si="7"/>
@@ -11147,7 +11147,7 @@
       </c>
       <c r="S26">
         <f t="shared" si="8"/>
-        <v>0.48885244864173755</v>
+        <v>0.55990512939623915</v>
       </c>
       <c r="T26">
         <f t="shared" si="9"/>
@@ -11155,11 +11155,11 @@
       </c>
       <c r="U26">
         <f t="shared" si="10"/>
-        <v>0.44745514441810891</v>
+        <v>0.50630509104027299</v>
       </c>
       <c r="V26">
         <f t="shared" si="11"/>
-        <v>0.28308613561629137</v>
+        <v>0.32082775242276018</v>
       </c>
       <c r="W26">
         <f t="shared" si="12"/>
@@ -11167,7 +11167,7 @@
       </c>
       <c r="X26">
         <f t="shared" si="13"/>
-        <v>31.948304613499666</v>
+        <v>31.837636493358048</v>
       </c>
       <c r="Y26">
         <f t="shared" si="14"/>
@@ -11179,11 +11179,11 @@
       </c>
       <c r="AA26">
         <f t="shared" si="16"/>
-        <v>73.534927194877952</v>
+        <v>74.520288543033303</v>
       </c>
       <c r="AB26">
         <f t="shared" si="17"/>
-        <v>3.6181965488918726</v>
+        <v>3.6666800541499764</v>
       </c>
       <c r="AC26">
         <f t="shared" si="18"/>
@@ -11191,11 +11191,11 @@
       </c>
       <c r="AD26">
         <f t="shared" si="19"/>
-        <v>1.1021077003121853</v>
+        <v>1.0536241950540814</v>
       </c>
       <c r="AE26">
         <f t="shared" si="20"/>
-        <v>-228.63854433000228</v>
+        <v>-247.39141910703117</v>
       </c>
       <c r="AF26">
         <f t="shared" si="21"/>
@@ -11207,7 +11207,7 @@
       </c>
       <c r="AH26">
         <f t="shared" si="23"/>
-        <v>25.724921596437611</v>
+        <v>6.9720468194087175</v>
       </c>
       <c r="AI26">
         <v>0</v>
@@ -11271,7 +11271,7 @@
       </c>
       <c r="BA26">
         <f t="shared" si="30"/>
-        <v>45.079934607965569</v>
+        <v>32.769395582938948</v>
       </c>
       <c r="BB26">
         <f t="shared" si="31"/>
@@ -11279,7 +11279,7 @@
       </c>
       <c r="BC26">
         <f t="shared" si="32"/>
-        <v>6.7452391260060543E-2</v>
+        <v>4.9163541965614899E-2</v>
       </c>
       <c r="BD26">
         <f t="shared" si="33"/>
@@ -11362,10 +11362,10 @@
         <v>414.98399999999998</v>
       </c>
       <c r="BZ26">
-        <v>471.65197974398802</v>
+        <v>457.093595948798</v>
       </c>
       <c r="CA26">
-        <v>36.441705567435903</v>
+        <v>36.9300211134872</v>
       </c>
       <c r="CB26">
         <v>30.448</v>
@@ -11881,22 +11881,22 @@
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>2.4404310343657096</v>
+        <v>4.1733688739459467</v>
       </c>
       <c r="K27">
         <v>1629735832.0999999</v>
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
-        <v>6.223090885880269E-3</v>
+        <v>5.3186502211703037E-3</v>
       </c>
       <c r="M27">
         <f t="shared" si="2"/>
-        <v>6.2230908858802687</v>
+        <v>5.3186502211703033</v>
       </c>
       <c r="N27">
         <f t="shared" si="3"/>
-        <v>13.040591632880302</v>
+        <v>22.924483908574768</v>
       </c>
       <c r="O27">
         <f t="shared" si="4"/>
@@ -11904,11 +11904,11 @@
       </c>
       <c r="P27">
         <f t="shared" si="5"/>
-        <v>379.10925419547965</v>
+        <v>339.25295773698554</v>
       </c>
       <c r="Q27">
         <f t="shared" si="6"/>
-        <v>37.644234721470539</v>
+        <v>33.686642648979372</v>
       </c>
       <c r="R27">
         <f t="shared" si="7"/>
@@ -11916,7 +11916,7 @@
       </c>
       <c r="S27">
         <f t="shared" si="8"/>
-        <v>0.77876589719227296</v>
+        <v>0.5758128370963872</v>
       </c>
       <c r="T27">
         <f t="shared" si="9"/>
@@ -11924,11 +11924,11 @@
       </c>
       <c r="U27">
         <f t="shared" si="10"/>
-        <v>0.67902371573212938</v>
+        <v>0.51927012172620313</v>
       </c>
       <c r="V27">
         <f t="shared" si="11"/>
-        <v>0.43228224105556662</v>
+        <v>0.32916004374128593</v>
       </c>
       <c r="W27">
         <f t="shared" si="12"/>
@@ -11936,7 +11936,7 @@
       </c>
       <c r="X27">
         <f t="shared" si="13"/>
-        <v>31.36746316543211</v>
+        <v>31.60295135436769</v>
       </c>
       <c r="Y27">
         <f t="shared" si="14"/>
@@ -11948,11 +11948,11 @@
       </c>
       <c r="AA27">
         <f t="shared" si="16"/>
-        <v>77.662071194679712</v>
+        <v>75.548688583072703</v>
       </c>
       <c r="AB27">
         <f t="shared" si="17"/>
-        <v>3.7849862614082506</v>
+        <v>3.6819871522294618</v>
       </c>
       <c r="AC27">
         <f t="shared" si="18"/>
@@ -11960,11 +11960,11 @@
       </c>
       <c r="AD27">
         <f t="shared" si="19"/>
-        <v>0.87134776975258532</v>
+        <v>0.97434687893137406</v>
       </c>
       <c r="AE27">
         <f t="shared" si="20"/>
-        <v>-274.43830806731984</v>
+        <v>-234.5524747536104</v>
       </c>
       <c r="AF27">
         <f t="shared" si="21"/>
@@ -11976,7 +11976,7 @@
       </c>
       <c r="AH27">
         <f t="shared" si="23"/>
-        <v>-31.938625420148867</v>
+        <v>7.9472078935605737</v>
       </c>
       <c r="AI27">
         <v>0</v>
@@ -12040,7 +12040,7 @@
       </c>
       <c r="BA27">
         <f t="shared" si="30"/>
-        <v>13.040591632880302</v>
+        <v>22.924483908574768</v>
       </c>
       <c r="BB27">
         <f t="shared" si="31"/>
@@ -12048,7 +12048,7 @@
       </c>
       <c r="BC27">
         <f t="shared" si="32"/>
-        <v>2.4418506213069568E-2</v>
+        <v>4.2478180870745626E-2</v>
       </c>
       <c r="BD27">
         <f t="shared" si="33"/>
@@ -12131,10 +12131,10 @@
         <v>414.99200000000002</v>
       </c>
       <c r="BZ27">
-        <v>433.73884963017002</v>
+        <v>445.14856992603399</v>
       </c>
       <c r="CA27">
-        <v>38.118010083605299</v>
+        <v>37.080722016721097</v>
       </c>
       <c r="CB27">
         <v>30.935300000000002</v>
@@ -12650,22 +12650,22 @@
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>5.2560057917734904</v>
+        <v>3.9328527663020236</v>
       </c>
       <c r="K28">
         <v>1629736622.5999999</v>
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
-        <v>2.8241493778931796E-3</v>
+        <v>4.0835453969499998E-3</v>
       </c>
       <c r="M28">
         <f t="shared" si="2"/>
-        <v>2.8241493778931797</v>
+        <v>4.08354539695</v>
       </c>
       <c r="N28">
         <f t="shared" si="3"/>
-        <v>30.713225661942495</v>
+        <v>22.068193583605478</v>
       </c>
       <c r="O28">
         <f t="shared" si="4"/>
@@ -12673,11 +12673,11 @@
       </c>
       <c r="P28">
         <f t="shared" si="5"/>
-        <v>183.72368073336941</v>
+        <v>309.84241591500734</v>
       </c>
       <c r="Q28">
         <f t="shared" si="6"/>
-        <v>18.243745237277839</v>
+        <v>30.767324479306421</v>
       </c>
       <c r="R28">
         <f t="shared" si="7"/>
@@ -12685,7 +12685,7 @@
       </c>
       <c r="S28">
         <f t="shared" si="8"/>
-        <v>0.22639788521701509</v>
+        <v>0.38052233427762583</v>
       </c>
       <c r="T28">
         <f t="shared" si="9"/>
@@ -12693,11 +12693,11 @@
       </c>
       <c r="U28">
         <f t="shared" si="10"/>
-        <v>0.21704526932765292</v>
+        <v>0.35487580031611471</v>
       </c>
       <c r="V28">
         <f t="shared" si="11"/>
-        <v>0.13646139349277642</v>
+        <v>0.22395740860415289</v>
       </c>
       <c r="W28">
         <f t="shared" si="12"/>
@@ -12705,7 +12705,7 @@
       </c>
       <c r="X28">
         <f t="shared" si="13"/>
-        <v>32.215703294659974</v>
+        <v>31.887300074380548</v>
       </c>
       <c r="Y28">
         <f t="shared" si="14"/>
@@ -12717,11 +12717,11 @@
       </c>
       <c r="AA28">
         <f t="shared" si="16"/>
-        <v>71.017592079859256</v>
+        <v>73.956515634094586</v>
       </c>
       <c r="AB28">
         <f t="shared" si="17"/>
-        <v>3.4817842629504137</v>
+        <v>3.6258710656914048</v>
       </c>
       <c r="AC28">
         <f t="shared" si="18"/>
@@ -12729,11 +12729,11 @@
       </c>
       <c r="AD28">
         <f t="shared" si="19"/>
-        <v>1.2387072892676079</v>
+        <v>1.0946204865266167</v>
       </c>
       <c r="AE28">
         <f t="shared" si="20"/>
-        <v>-124.54498756508922</v>
+        <v>-180.08435200549499</v>
       </c>
       <c r="AF28">
         <f t="shared" si="21"/>
@@ -12745,7 +12745,7 @@
       </c>
       <c r="AH28">
         <f t="shared" si="23"/>
-        <v>70.783842154660874</v>
+        <v>15.244477714255098</v>
       </c>
       <c r="AI28">
         <v>0</v>
@@ -12809,7 +12809,7 @@
       </c>
       <c r="BA28">
         <f t="shared" si="30"/>
-        <v>30.713225661942495</v>
+        <v>22.068193583605478</v>
       </c>
       <c r="BB28">
         <f t="shared" si="31"/>
@@ -12817,7 +12817,7 @@
       </c>
       <c r="BC28">
         <f t="shared" si="32"/>
-        <v>7.3700030556750701E-2</v>
+        <v>5.3171429381093926E-2</v>
       </c>
       <c r="BD28">
         <f t="shared" si="33"/>
@@ -12900,10 +12900,10 @@
         <v>414.988</v>
       </c>
       <c r="BZ28">
-        <v>453.24635416464599</v>
+        <v>443.50047083292901</v>
       </c>
       <c r="CA28">
-        <v>35.063316878690401</v>
+        <v>36.5143433757381</v>
       </c>
       <c r="CB28">
         <v>31.793500000000002</v>
@@ -13419,22 +13419,22 @@
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>5.1685386744600681</v>
+        <v>3.0593736067516009</v>
       </c>
       <c r="K29">
         <v>1629737091</v>
       </c>
       <c r="L29">
         <f t="shared" si="1"/>
-        <v>2.5633287876024517E-3</v>
+        <v>3.6702683115789956E-3</v>
       </c>
       <c r="M29">
         <f t="shared" si="2"/>
-        <v>2.5633287876024515</v>
+        <v>3.6702683115789956</v>
       </c>
       <c r="N29">
         <f t="shared" si="3"/>
-        <v>29.914445186549564</v>
+        <v>17.09159337697869</v>
       </c>
       <c r="O29">
         <f t="shared" si="4"/>
@@ -13442,11 +13442,11 @@
       </c>
       <c r="P29">
         <f t="shared" si="5"/>
-        <v>174.817798207772</v>
+        <v>325.00535620487011</v>
       </c>
       <c r="Q29">
         <f t="shared" si="6"/>
-        <v>17.357620024862886</v>
+        <v>32.269709016381761</v>
       </c>
       <c r="R29">
         <f t="shared" si="7"/>
@@ -13454,7 +13454,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="8"/>
-        <v>0.21129944133256515</v>
+        <v>0.34628276053440049</v>
       </c>
       <c r="T29">
         <f t="shared" si="9"/>
@@ -13462,11 +13462,11 @@
       </c>
       <c r="U29">
         <f t="shared" si="10"/>
-        <v>0.20314034250665475</v>
+        <v>0.32493516231919678</v>
       </c>
       <c r="V29">
         <f t="shared" si="11"/>
-        <v>0.12766952608304719</v>
+        <v>0.20489271102815107</v>
       </c>
       <c r="W29">
         <f t="shared" si="12"/>
@@ -13474,7 +13474,7 @@
       </c>
       <c r="X29">
         <f t="shared" si="13"/>
-        <v>32.146938956579412</v>
+        <v>31.858697730674191</v>
       </c>
       <c r="Y29">
         <f t="shared" si="14"/>
@@ -13486,11 +13486,11 @@
       </c>
       <c r="AA29">
         <f t="shared" si="16"/>
-        <v>71.711413398964709</v>
+        <v>74.29360427952814</v>
       </c>
       <c r="AB29">
         <f t="shared" si="17"/>
-        <v>3.5169903673834177</v>
+        <v>3.6436304658453174</v>
       </c>
       <c r="AC29">
         <f t="shared" si="18"/>
@@ -13498,11 +13498,11 @@
       </c>
       <c r="AD29">
         <f t="shared" si="19"/>
-        <v>1.2009330218566463</v>
+        <v>1.0742929233947467</v>
       </c>
       <c r="AE29">
         <f t="shared" si="20"/>
-        <v>-113.04279953326812</v>
+        <v>-161.8588325406337</v>
       </c>
       <c r="AF29">
         <f t="shared" si="21"/>
@@ -13514,7 +13514,7 @@
       </c>
       <c r="AH29">
         <f t="shared" si="23"/>
-        <v>60.862600238502282</v>
+        <v>12.046567231136706</v>
       </c>
       <c r="AI29">
         <v>1</v>
@@ -13578,7 +13578,7 @@
       </c>
       <c r="BA29">
         <f t="shared" si="30"/>
-        <v>29.914445186549564</v>
+        <v>17.09159337697869</v>
       </c>
       <c r="BB29">
         <f t="shared" si="31"/>
@@ -13586,7 +13586,7 @@
       </c>
       <c r="BC29">
         <f t="shared" si="32"/>
-        <v>0.10249184206628317</v>
+        <v>5.9028546803018396E-2</v>
       </c>
       <c r="BD29">
         <f t="shared" si="33"/>
@@ -13669,10 +13669,10 @@
         <v>415.05099999999999</v>
       </c>
       <c r="BZ29">
-        <v>452.21923059183501</v>
+        <v>437.38544611836699</v>
       </c>
       <c r="CA29">
-        <v>35.421475493946303</v>
+        <v>36.696935098789197</v>
       </c>
       <c r="CB29">
         <v>32.454900000000002</v>
@@ -14188,22 +14188,22 @@
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>4.252050735617142</v>
+        <v>1.9380511599206938</v>
       </c>
       <c r="K30">
         <v>1629737500.5</v>
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
-        <v>3.2171090294902541E-3</v>
+        <v>3.3600535704715571E-3</v>
       </c>
       <c r="M30">
         <f t="shared" si="2"/>
-        <v>3.217109029490254</v>
+        <v>3.3600535704715573</v>
       </c>
       <c r="N30">
         <f t="shared" si="3"/>
-        <v>23.731226153731946</v>
+        <v>10.768249624445012</v>
       </c>
       <c r="O30">
         <f t="shared" si="4"/>
@@ -14211,11 +14211,11 @@
       </c>
       <c r="P30">
         <f t="shared" si="5"/>
-        <v>275.61621903917455</v>
+        <v>351.24917376029549</v>
       </c>
       <c r="Q30">
         <f t="shared" si="6"/>
-        <v>27.366110782779828</v>
+        <v>34.875755262130944</v>
       </c>
       <c r="R30">
         <f t="shared" si="7"/>
@@ -14223,7 +14223,7 @@
       </c>
       <c r="S30">
         <f t="shared" si="8"/>
-        <v>0.29899258639897541</v>
+        <v>0.31812532667855031</v>
       </c>
       <c r="T30">
         <f t="shared" si="9"/>
@@ -14231,11 +14231,11 @@
       </c>
       <c r="U30">
         <f t="shared" si="10"/>
-        <v>0.28293304987047724</v>
+        <v>0.30001155051170675</v>
       </c>
       <c r="V30">
         <f t="shared" si="11"/>
-        <v>0.17820412463895147</v>
+        <v>0.18904866755823002</v>
       </c>
       <c r="W30">
         <f t="shared" si="12"/>
@@ -14243,7 +14243,7 @@
       </c>
       <c r="X30">
         <f t="shared" si="13"/>
-        <v>31.823774333092523</v>
+        <v>31.78655362881312</v>
       </c>
       <c r="Y30">
         <f t="shared" si="14"/>
@@ -14255,11 +14255,11 @@
       </c>
       <c r="AA30">
         <f t="shared" si="16"/>
-        <v>74.361174294720499</v>
+        <v>74.694410177232584</v>
       </c>
       <c r="AB30">
         <f t="shared" si="17"/>
-        <v>3.645607471648745</v>
+        <v>3.6619445888961493</v>
       </c>
       <c r="AC30">
         <f t="shared" si="18"/>
@@ -14267,11 +14267,11 @@
       </c>
       <c r="AD30">
         <f t="shared" si="19"/>
-        <v>1.081390183476552</v>
+        <v>1.0650530662291477</v>
       </c>
       <c r="AE30">
         <f t="shared" si="20"/>
-        <v>-141.87450820052021</v>
+        <v>-148.17836245779566</v>
       </c>
       <c r="AF30">
         <f t="shared" si="21"/>
@@ -14283,7 +14283,7 @@
       </c>
       <c r="AH30">
         <f t="shared" si="23"/>
-        <v>0.39400678813797185</v>
+        <v>-5.9098474691374747</v>
       </c>
       <c r="AI30">
         <v>1</v>
@@ -14347,7 +14347,7 @@
       </c>
       <c r="BA30">
         <f t="shared" si="30"/>
-        <v>23.731226153731946</v>
+        <v>10.768249624445012</v>
       </c>
       <c r="BB30">
         <f t="shared" si="31"/>
@@ -14355,7 +14355,7 @@
       </c>
       <c r="BC30">
         <f t="shared" si="32"/>
-        <v>0.14266501420367814</v>
+        <v>6.578329908944304E-2</v>
       </c>
       <c r="BD30">
         <f t="shared" si="33"/>
@@ -14438,10 +14438,10 @@
         <v>415.01900000000001</v>
       </c>
       <c r="BZ30">
-        <v>445.092530031124</v>
+        <v>429.61130600622499</v>
       </c>
       <c r="CA30">
-        <v>36.716527072932003</v>
+        <v>36.881065414586402</v>
       </c>
       <c r="CB30">
         <v>32.9985</v>
@@ -14957,22 +14957,22 @@
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>11.620308654112398</v>
+        <v>8.663128143909459</v>
       </c>
       <c r="K31">
         <v>1629738760.0999999</v>
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
-        <v>8.5337190897203843E-3</v>
+        <v>8.0808435993445869E-3</v>
       </c>
       <c r="M31">
         <f t="shared" si="2"/>
-        <v>8.5337190897203836</v>
+        <v>8.0808435993445862</v>
       </c>
       <c r="N31">
         <f t="shared" si="3"/>
-        <v>63.484712959998966</v>
+        <v>47.950459806596754</v>
       </c>
       <c r="O31">
         <f t="shared" si="4"/>
@@ -14980,11 +14980,11 @@
       </c>
       <c r="P31">
         <f t="shared" si="5"/>
-        <v>261.31212276062706</v>
+        <v>285.27705824493069</v>
       </c>
       <c r="Q31">
         <f t="shared" si="6"/>
-        <v>25.946212099366715</v>
+        <v>28.32573928109252</v>
       </c>
       <c r="R31">
         <f t="shared" si="7"/>
@@ -14992,7 +14992,7 @@
       </c>
       <c r="S31">
         <f t="shared" si="8"/>
-        <v>0.77833915881784599</v>
+        <v>0.6974766529312918</v>
       </c>
       <c r="T31">
         <f t="shared" si="9"/>
@@ -15000,11 +15000,11 @@
       </c>
       <c r="U31">
         <f t="shared" si="10"/>
-        <v>0.6787996769804705</v>
+        <v>0.61639701271715275</v>
       </c>
       <c r="V31">
         <f t="shared" si="11"/>
-        <v>0.43212777233712157</v>
+        <v>0.39174456361412024</v>
       </c>
       <c r="W31">
         <f t="shared" si="12"/>
@@ -15012,7 +15012,7 @@
       </c>
       <c r="X31">
         <f t="shared" si="13"/>
-        <v>33.231785547676296</v>
+        <v>33.349471783333591</v>
       </c>
       <c r="Y31">
         <f t="shared" si="14"/>
@@ -15024,11 +15024,11 @@
       </c>
       <c r="AA31">
         <f t="shared" si="16"/>
-        <v>75.943915568110441</v>
+        <v>74.959459086181468</v>
       </c>
       <c r="AB31">
         <f t="shared" si="17"/>
-        <v>3.9580507999800743</v>
+        <v>3.9067428217609379</v>
       </c>
       <c r="AC31">
         <f t="shared" si="18"/>
@@ -15036,11 +15036,11 @@
       </c>
       <c r="AD31">
         <f t="shared" si="19"/>
-        <v>1.1910310142133671</v>
+        <v>1.2423389924325035</v>
       </c>
       <c r="AE31">
         <f t="shared" si="20"/>
-        <v>-376.33701185666894</v>
+        <v>-356.3652027310963</v>
       </c>
       <c r="AF31">
         <f t="shared" si="21"/>
@@ -15052,7 +15052,7 @@
       </c>
       <c r="AH31">
         <f t="shared" si="23"/>
-        <v>-18.163604237158431</v>
+        <v>1.8082048884142026</v>
       </c>
       <c r="AI31">
         <v>1</v>
@@ -15116,7 +15116,7 @@
       </c>
       <c r="BA31">
         <f t="shared" si="30"/>
-        <v>63.484712959998966</v>
+        <v>47.950459806596754</v>
       </c>
       <c r="BB31">
         <f t="shared" si="31"/>
@@ -15124,7 +15124,7 @@
       </c>
       <c r="BC31">
         <f t="shared" si="32"/>
-        <v>3.7956840062654193E-2</v>
+        <v>2.8716151743085346E-2</v>
       </c>
       <c r="BD31">
         <f t="shared" si="33"/>
@@ -15207,10 +15207,10 @@
         <v>414.90100000000001</v>
       </c>
       <c r="BZ31">
-        <v>495.325482441151</v>
+        <v>476.46029648822997</v>
       </c>
       <c r="CA31">
-        <v>39.862722642371203</v>
+        <v>39.345984528474197</v>
       </c>
       <c r="CB31">
         <v>30.031199999999998</v>
@@ -15726,22 +15726,22 @@
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>2.7502189182858952</v>
+        <v>5.4943226355247425</v>
       </c>
       <c r="K32">
         <v>1629739435.5999999</v>
       </c>
       <c r="L32">
         <f t="shared" si="1"/>
-        <v>6.5055274437569267E-3</v>
+        <v>5.9397133313920502E-3</v>
       </c>
       <c r="M32">
         <f t="shared" si="2"/>
-        <v>6.505527443756927</v>
+        <v>5.93971333139205</v>
       </c>
       <c r="N32">
         <f t="shared" si="3"/>
-        <v>14.895325164160409</v>
+        <v>30.250627493665597</v>
       </c>
       <c r="O32">
         <f t="shared" si="4"/>
@@ -15749,11 +15749,11 @@
       </c>
       <c r="P32">
         <f t="shared" si="5"/>
-        <v>368.53298529821723</v>
+        <v>314.41741099767609</v>
       </c>
       <c r="Q32">
         <f t="shared" si="6"/>
-        <v>36.5924718892078</v>
+        <v>31.219214378055877</v>
       </c>
       <c r="R32">
         <f t="shared" si="7"/>
@@ -15761,7 +15761,7 @@
       </c>
       <c r="S32">
         <f t="shared" si="8"/>
-        <v>0.66553621827034393</v>
+        <v>0.56278917677130802</v>
       </c>
       <c r="T32">
         <f t="shared" si="9"/>
@@ -15769,11 +15769,11 @@
       </c>
       <c r="U32">
         <f t="shared" si="10"/>
-        <v>0.59117290396221756</v>
+        <v>0.50861620357865633</v>
       </c>
       <c r="V32">
         <f t="shared" si="11"/>
-        <v>0.37546958159778598</v>
+        <v>0.32231669268058805</v>
       </c>
       <c r="W32">
         <f t="shared" si="12"/>
@@ -15781,7 +15781,7 @@
       </c>
       <c r="X32">
         <f t="shared" si="13"/>
-        <v>32.682122417863788</v>
+        <v>32.829427268327272</v>
       </c>
       <c r="Y32">
         <f t="shared" si="14"/>
@@ -15793,11 +15793,11 @@
       </c>
       <c r="AA32">
         <f t="shared" si="16"/>
-        <v>76.622620638280765</v>
+        <v>75.373641080309199</v>
       </c>
       <c r="AB32">
         <f t="shared" si="17"/>
-        <v>3.9425317768067583</v>
+        <v>3.8782669219262296</v>
       </c>
       <c r="AC32">
         <f t="shared" si="18"/>
@@ -15805,11 +15805,11 @@
       </c>
       <c r="AD32">
         <f t="shared" si="19"/>
-        <v>1.0435287167374154</v>
+        <v>1.1077935716179441</v>
       </c>
       <c r="AE32">
         <f t="shared" si="20"/>
-        <v>-286.89376026968046</v>
+        <v>-261.94135791438941</v>
       </c>
       <c r="AF32">
         <f t="shared" si="21"/>
@@ -15821,7 +15821,7 @@
       </c>
       <c r="AH32">
         <f t="shared" si="23"/>
-        <v>-14.227268369564939</v>
+        <v>10.725133985726103</v>
       </c>
       <c r="AI32">
         <v>3</v>
@@ -15885,7 +15885,7 @@
       </c>
       <c r="BA32">
         <f t="shared" si="30"/>
-        <v>14.895325164160409</v>
+        <v>30.250627493665597</v>
       </c>
       <c r="BB32">
         <f t="shared" si="31"/>
@@ -15893,7 +15893,7 @@
       </c>
       <c r="BC32">
         <f t="shared" si="32"/>
-        <v>1.6451098875758054E-2</v>
+        <v>3.3049801739583114E-2</v>
       </c>
       <c r="BD32">
         <f t="shared" si="33"/>
@@ -15976,10 +15976,10 @@
         <v>414.99200000000002</v>
       </c>
       <c r="BZ32">
-        <v>436.10038114801</v>
+        <v>454.24007622960198</v>
       </c>
       <c r="CA32">
-        <v>39.706336585810099</v>
+        <v>39.059107317162002</v>
       </c>
       <c r="CB32">
         <v>32.2117</v>
@@ -16495,22 +16495,22 @@
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>2.9694624839751311</v>
+        <v>4.6451345497687537</v>
       </c>
       <c r="K33">
         <v>1629739945.5</v>
       </c>
       <c r="L33">
         <f t="shared" si="1"/>
-        <v>5.6996046639291881E-3</v>
+        <v>4.9933674765488545E-3</v>
       </c>
       <c r="M33">
         <f t="shared" si="2"/>
-        <v>5.699604663929188</v>
+        <v>4.9933674765488547</v>
       </c>
       <c r="N33">
         <f t="shared" si="3"/>
-        <v>15.950235455082842</v>
+        <v>25.472459547518479</v>
       </c>
       <c r="O33">
         <f t="shared" si="4"/>
@@ -16518,11 +16518,11 @@
       </c>
       <c r="P33">
         <f t="shared" si="5"/>
-        <v>363.68553171219611</v>
+        <v>319.46266548477399</v>
       </c>
       <c r="Q33">
         <f t="shared" si="6"/>
-        <v>36.11334303199461</v>
+        <v>31.722089053838772</v>
       </c>
       <c r="R33">
         <f t="shared" si="7"/>
@@ -16530,7 +16530,7 @@
       </c>
       <c r="S33">
         <f t="shared" si="8"/>
-        <v>0.62415981809785392</v>
+        <v>0.4941280994823527</v>
       </c>
       <c r="T33">
         <f t="shared" si="9"/>
@@ -16538,11 +16538,11 @@
       </c>
       <c r="U33">
         <f t="shared" si="10"/>
-        <v>0.55825575654408344</v>
+        <v>0.4518287058674233</v>
       </c>
       <c r="V33">
         <f t="shared" si="11"/>
-        <v>0.35424941339244659</v>
+        <v>0.28589101357749319</v>
       </c>
       <c r="W33">
         <f t="shared" si="12"/>
@@ -16550,7 +16550,7 @@
       </c>
       <c r="X33">
         <f t="shared" si="13"/>
-        <v>32.375829304099149</v>
+        <v>32.559754966192038</v>
       </c>
       <c r="Y33">
         <f t="shared" si="14"/>
@@ -16562,11 +16562,11 @@
       </c>
       <c r="AA33">
         <f t="shared" si="16"/>
-        <v>77.256081752379387</v>
+        <v>75.674463480621228</v>
       </c>
       <c r="AB33">
         <f t="shared" si="17"/>
-        <v>3.923435663816357</v>
+        <v>3.8431134756700693</v>
       </c>
       <c r="AC33">
         <f t="shared" si="18"/>
@@ -16574,11 +16574,11 @@
       </c>
       <c r="AD33">
         <f t="shared" si="19"/>
-        <v>0.96879958664828791</v>
+        <v>1.0491217747945756</v>
       </c>
       <c r="AE33">
         <f t="shared" si="20"/>
-        <v>-251.35256567927721</v>
+        <v>-220.20750571580447</v>
       </c>
       <c r="AF33">
         <f t="shared" si="21"/>
@@ -16590,7 +16590,7 @@
       </c>
       <c r="AH33">
         <f t="shared" si="23"/>
-        <v>-9.0133751021932227</v>
+        <v>22.13168486127951</v>
       </c>
       <c r="AI33">
         <v>4</v>
@@ -16654,7 +16654,7 @@
       </c>
       <c r="BA33">
         <f t="shared" si="30"/>
-        <v>15.950235455082842</v>
+        <v>25.472459547518479</v>
       </c>
       <c r="BB33">
         <f t="shared" si="31"/>
@@ -16662,7 +16662,7 @@
       </c>
       <c r="BC33">
         <f t="shared" si="32"/>
-        <v>2.4177698216798237E-2</v>
+        <v>3.8324815805169117E-2</v>
       </c>
       <c r="BD33">
         <f t="shared" si="33"/>
@@ -16745,10 +16745,10 @@
         <v>414.97500000000002</v>
       </c>
       <c r="BZ33">
-        <v>436.94661559330001</v>
+        <v>448.01812311866001</v>
       </c>
       <c r="CA33">
-        <v>39.511622733721602</v>
+        <v>38.7027245467443</v>
       </c>
       <c r="CB33">
         <v>32.944400000000002</v>
@@ -17264,22 +17264,22 @@
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>7.1820565003474357</v>
+        <v>4.7998960140120337</v>
       </c>
       <c r="K34">
         <v>1629740324.5</v>
       </c>
       <c r="L34">
         <f t="shared" si="1"/>
-        <v>6.0642032311220779E-3</v>
+        <v>4.7851499220024516E-3</v>
       </c>
       <c r="M34">
         <f t="shared" si="2"/>
-        <v>6.0642032311220779</v>
+        <v>4.7851499220024518</v>
       </c>
       <c r="N34">
         <f t="shared" si="3"/>
-        <v>38.02938354519177</v>
+        <v>26.383034815824359</v>
       </c>
       <c r="O34">
         <f t="shared" si="4"/>
@@ -17287,11 +17287,11 @@
       </c>
       <c r="P34">
         <f t="shared" si="5"/>
-        <v>314.6540479256596</v>
+        <v>311.47869496356742</v>
       </c>
       <c r="Q34">
         <f t="shared" si="6"/>
-        <v>31.24304922341129</v>
+        <v>30.927757843718663</v>
       </c>
       <c r="R34">
         <f t="shared" si="7"/>
@@ -17299,7 +17299,7 @@
       </c>
       <c r="S34">
         <f t="shared" si="8"/>
-        <v>0.7160787009495444</v>
+        <v>0.46767888505192534</v>
       </c>
       <c r="T34">
         <f t="shared" si="9"/>
@@ -17307,11 +17307,11 @@
       </c>
       <c r="U34">
         <f t="shared" si="10"/>
-        <v>0.63087070808867041</v>
+        <v>0.42965616684850733</v>
       </c>
       <c r="V34">
         <f t="shared" si="11"/>
-        <v>0.40110172043640108</v>
+        <v>0.2716932224999698</v>
       </c>
       <c r="W34">
         <f t="shared" si="12"/>
@@ -17319,7 +17319,7 @@
       </c>
       <c r="X34">
         <f t="shared" si="13"/>
-        <v>32.08405694979205</v>
+        <v>32.41667467981955</v>
       </c>
       <c r="Y34">
         <f t="shared" si="14"/>
@@ -17331,11 +17331,11 @@
       </c>
       <c r="AA34">
         <f t="shared" si="16"/>
-        <v>78.371614072718998</v>
+        <v>75.498154840474683</v>
       </c>
       <c r="AB34">
         <f t="shared" si="17"/>
-        <v>3.9673446998348716</v>
+        <v>3.8218838287003525</v>
       </c>
       <c r="AC34">
         <f t="shared" si="18"/>
@@ -17343,11 +17343,11 @@
       </c>
       <c r="AD34">
         <f t="shared" si="19"/>
-        <v>0.91193185867456261</v>
+        <v>1.0573927298090817</v>
       </c>
       <c r="AE34">
         <f t="shared" si="20"/>
-        <v>-267.43136249248363</v>
+        <v>-211.02511156030812</v>
       </c>
       <c r="AF34">
         <f t="shared" si="21"/>
@@ -17359,7 +17359,7 @@
       </c>
       <c r="AH34">
         <f t="shared" si="23"/>
-        <v>-50.534895567641215</v>
+        <v>5.8713553645342955</v>
       </c>
       <c r="AI34">
         <v>4</v>
@@ -17423,7 +17423,7 @@
       </c>
       <c r="BA34">
         <f t="shared" si="30"/>
-        <v>38.02938354519177</v>
+        <v>26.383034815824359</v>
       </c>
       <c r="BB34">
         <f t="shared" si="31"/>
@@ -17431,7 +17431,7 @@
       </c>
       <c r="BC34">
         <f t="shared" si="32"/>
-        <v>7.0081752414032458E-2</v>
+        <v>4.880048383901766E-2</v>
       </c>
       <c r="BD34">
         <f t="shared" si="33"/>
@@ -17514,10 +17514,10 @@
         <v>414.98200000000003</v>
       </c>
       <c r="BZ34">
-        <v>463.63165371532301</v>
+        <v>449.02073074306497</v>
       </c>
       <c r="CA34">
-        <v>39.955801381384902</v>
+        <v>38.490840276276998</v>
       </c>
       <c r="CB34">
         <v>32.970300000000002</v>
@@ -18033,22 +18033,22 @@
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>2.0459691425893616</v>
+        <v>3.0848016081957321</v>
       </c>
       <c r="K35">
         <v>1629740707.5</v>
       </c>
       <c r="L35">
         <f t="shared" si="1"/>
-        <v>5.3052482779682979E-3</v>
+        <v>4.3920194321675991E-3</v>
       </c>
       <c r="M35">
         <f t="shared" si="2"/>
-        <v>5.3052482779682979</v>
+        <v>4.3920194321675989</v>
       </c>
       <c r="N35">
         <f t="shared" si="3"/>
-        <v>10.981154125870031</v>
+        <v>17.009070307591315</v>
       </c>
       <c r="O35">
         <f t="shared" si="4"/>
@@ -18056,11 +18056,11 @@
       </c>
       <c r="P35">
         <f t="shared" si="5"/>
-        <v>375.7108977837579</v>
+        <v>339.67571223369896</v>
       </c>
       <c r="Q35">
         <f t="shared" si="6"/>
-        <v>37.30784286574648</v>
+        <v>33.729572849971241</v>
       </c>
       <c r="R35">
         <f t="shared" si="7"/>
@@ -18068,7 +18068,7 @@
       </c>
       <c r="S35">
         <f t="shared" si="8"/>
-        <v>0.58242360408500171</v>
+        <v>0.42357515225558828</v>
       </c>
       <c r="T35">
         <f t="shared" si="9"/>
@@ -18076,11 +18076,11 @@
       </c>
       <c r="U35">
         <f t="shared" si="10"/>
-        <v>0.52477709123160809</v>
+        <v>0.39217834749359176</v>
       </c>
       <c r="V35">
         <f t="shared" si="11"/>
-        <v>0.33268823627653044</v>
+        <v>0.2477381278841595</v>
       </c>
       <c r="W35">
         <f t="shared" si="12"/>
@@ -18088,7 +18088,7 @@
       </c>
       <c r="X35">
         <f t="shared" si="13"/>
-        <v>32.124494661983803</v>
+        <v>32.361595095466392</v>
       </c>
       <c r="Y35">
         <f t="shared" si="14"/>
@@ -18100,11 +18100,11 @@
       </c>
       <c r="AA35">
         <f t="shared" si="16"/>
-        <v>77.32559271383407</v>
+        <v>75.26946474357409</v>
       </c>
       <c r="AB35">
         <f t="shared" si="17"/>
-        <v>3.9106562842552957</v>
+        <v>3.8066698874372635</v>
       </c>
       <c r="AC35">
         <f t="shared" si="18"/>
@@ -18112,11 +18112,11 @@
       </c>
       <c r="AD35">
         <f t="shared" si="19"/>
-        <v>0.95948448997924052</v>
+        <v>1.0634708867972726</v>
       </c>
       <c r="AE35">
         <f t="shared" si="20"/>
-        <v>-233.96144905840194</v>
+        <v>-193.68805695859112</v>
       </c>
       <c r="AF35">
         <f t="shared" si="21"/>
@@ -18128,7 +18128,7 @@
       </c>
       <c r="AH35">
         <f t="shared" si="23"/>
-        <v>-38.110182689535677</v>
+        <v>2.163209410275158</v>
       </c>
       <c r="AI35">
         <v>4</v>
@@ -18192,7 +18192,7 @@
       </c>
       <c r="BA35">
         <f t="shared" si="30"/>
-        <v>10.981154125870031</v>
+        <v>17.009070307591315</v>
       </c>
       <c r="BB35">
         <f t="shared" si="31"/>
@@ -18200,7 +18200,7 @@
       </c>
       <c r="BC35">
         <f t="shared" si="32"/>
-        <v>2.6840702734636887E-2</v>
+        <v>4.1152905894799419E-2</v>
       </c>
       <c r="BD35">
         <f t="shared" si="33"/>
@@ -18283,10 +18283,10 @@
         <v>415.02300000000002</v>
       </c>
       <c r="BZ35">
-        <v>430.84260829675799</v>
+        <v>437.62132165935202</v>
       </c>
       <c r="CA35">
-        <v>39.382501657050803</v>
+        <v>38.335300331410203</v>
       </c>
       <c r="CB35">
         <v>33.2669</v>
@@ -18802,22 +18802,22 @@
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>4.9899201418353201</v>
+        <v>2.6571160781555339</v>
       </c>
       <c r="K36">
         <v>1629741908.0999999</v>
       </c>
       <c r="L36">
         <f t="shared" si="1"/>
-        <v>1.5939231779450677E-3</v>
+        <v>1.7730893052713774E-3</v>
       </c>
       <c r="M36">
         <f t="shared" si="2"/>
-        <v>1.5939231779450678</v>
+        <v>1.7730893052713774</v>
       </c>
       <c r="N36">
         <f t="shared" si="3"/>
-        <v>27.698864361308157</v>
+        <v>14.666531035139538</v>
       </c>
       <c r="O36">
         <f t="shared" si="4"/>
@@ -18825,11 +18825,11 @@
       </c>
       <c r="P36">
         <f t="shared" si="5"/>
-        <v>85.585698242220801</v>
+        <v>257.14739233546601</v>
       </c>
       <c r="Q36">
         <f t="shared" si="6"/>
-        <v>8.4959845976968698</v>
+        <v>25.526698145722147</v>
       </c>
       <c r="R36">
         <f t="shared" si="7"/>
@@ -18837,7 +18837,7 @@
       </c>
       <c r="S36">
         <f t="shared" si="8"/>
-        <v>0.13959987323524742</v>
+        <v>0.15874793213164212</v>
       </c>
       <c r="T36">
         <f t="shared" si="9"/>
@@ -18845,11 +18845,11 @@
       </c>
       <c r="U36">
         <f t="shared" si="10"/>
-        <v>0.13598395567579599</v>
+        <v>0.154089859050278</v>
       </c>
       <c r="V36">
         <f t="shared" si="11"/>
-        <v>8.5307047108875017E-2</v>
+        <v>9.6713286277727128E-2</v>
       </c>
       <c r="W36">
         <f t="shared" si="12"/>
@@ -18857,7 +18857,7 @@
       </c>
       <c r="X36">
         <f t="shared" si="13"/>
-        <v>32.198254844986458</v>
+        <v>32.151549648230585</v>
       </c>
       <c r="Y36">
         <f t="shared" si="14"/>
@@ -18869,11 +18869,11 @@
       </c>
       <c r="AA36">
         <f t="shared" si="16"/>
-        <v>74.754230180934044</v>
+        <v>75.177393407995751</v>
       </c>
       <c r="AB36">
         <f t="shared" si="17"/>
-        <v>3.6248398324352249</v>
+        <v>3.6453590581347268</v>
       </c>
       <c r="AC36">
         <f t="shared" si="18"/>
@@ -18881,11 +18881,11 @@
       </c>
       <c r="AD36">
         <f t="shared" si="19"/>
-        <v>1.114548984920861</v>
+        <v>1.094029759221359</v>
       </c>
       <c r="AE36">
         <f t="shared" si="20"/>
-        <v>-70.292012147377477</v>
+        <v>-78.193238362467739</v>
       </c>
       <c r="AF36">
         <f t="shared" si="21"/>
@@ -18897,7 +18897,7 @@
       </c>
       <c r="AH36">
         <f t="shared" si="23"/>
-        <v>55.944729880069069</v>
+        <v>48.043503664978807</v>
       </c>
       <c r="AI36">
         <v>4</v>
@@ -18961,7 +18961,7 @@
       </c>
       <c r="BA36">
         <f t="shared" si="30"/>
-        <v>27.698864361308157</v>
+        <v>14.666531035139538</v>
       </c>
       <c r="BB36">
         <f t="shared" si="31"/>
@@ -18969,7 +18969,7 @@
       </c>
       <c r="BC36">
         <f t="shared" si="32"/>
-        <v>9.4963337776934123E-2</v>
+        <v>5.0798721900180956E-2</v>
       </c>
       <c r="BD36">
         <f t="shared" si="33"/>
@@ -19052,10 +19052,10 @@
         <v>414.95800000000003</v>
       </c>
       <c r="BZ36">
-        <v>448.989513886125</v>
+        <v>433.44030277722499</v>
       </c>
       <c r="CA36">
-        <v>36.515420256209403</v>
+        <v>36.722124051241899</v>
       </c>
       <c r="CB36">
         <v>34.672600000000003</v>
@@ -19571,22 +19571,22 @@
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>3.3308724398931702</v>
+        <v>1.6597754987420892</v>
       </c>
       <c r="K37">
         <v>1629742488.0999999</v>
       </c>
       <c r="L37">
         <f t="shared" si="1"/>
-        <v>1.3770047460635335E-3</v>
+        <v>2.3568452688000493E-3</v>
       </c>
       <c r="M37">
         <f t="shared" si="2"/>
-        <v>1.3770047460635335</v>
+        <v>2.3568452688000492</v>
       </c>
       <c r="N37">
         <f t="shared" si="3"/>
-        <v>19.198739823302532</v>
+        <v>9.2760308462576919</v>
       </c>
       <c r="O37">
         <f t="shared" si="4"/>
@@ -19594,11 +19594,11 @@
       </c>
       <c r="P37">
         <f t="shared" si="5"/>
-        <v>115.23513069178841</v>
+        <v>332.36409557562177</v>
       </c>
       <c r="Q37">
         <f t="shared" si="6"/>
-        <v>11.43903243177119</v>
+        <v>32.992748353925023</v>
       </c>
       <c r="R37">
         <f t="shared" si="7"/>
@@ -19606,7 +19606,7 @@
       </c>
       <c r="S37">
         <f t="shared" si="8"/>
-        <v>0.10621899674744126</v>
+        <v>0.20308446656723356</v>
       </c>
       <c r="T37">
         <f t="shared" si="9"/>
@@ -19614,11 +19614,11 @@
       </c>
       <c r="U37">
         <f t="shared" si="10"/>
-        <v>0.10411569509327656</v>
+        <v>0.19554244842922613</v>
       </c>
       <c r="V37">
         <f t="shared" si="11"/>
-        <v>6.5257813810781024E-2</v>
+        <v>0.12286831452229784</v>
       </c>
       <c r="W37">
         <f t="shared" si="12"/>
@@ -19626,7 +19626,7 @@
       </c>
       <c r="X37">
         <f t="shared" si="13"/>
-        <v>32.547425138567533</v>
+        <v>32.29255740728366</v>
       </c>
       <c r="Y37">
         <f t="shared" si="14"/>
@@ -19638,11 +19638,11 @@
       </c>
       <c r="AA37">
         <f t="shared" si="16"/>
-        <v>72.005003438094604</v>
+        <v>74.261644566419463</v>
       </c>
       <c r="AB37">
         <f t="shared" si="17"/>
-        <v>3.5790333940854975</v>
+        <v>3.6912005154117975</v>
       </c>
       <c r="AC37">
         <f t="shared" si="18"/>
@@ -19650,11 +19650,11 @@
       </c>
       <c r="AD37">
         <f t="shared" si="19"/>
-        <v>1.2572266051769923</v>
+        <v>1.1450594838506922</v>
       </c>
       <c r="AE37">
         <f t="shared" si="20"/>
-        <v>-60.725909301401828</v>
+        <v>-103.93687635408217</v>
       </c>
       <c r="AF37">
         <f t="shared" si="21"/>
@@ -19666,7 +19666,7 @@
       </c>
       <c r="AH37">
         <f t="shared" si="23"/>
-        <v>54.633654821688985</v>
+        <v>11.422687769008647</v>
       </c>
       <c r="AI37">
         <v>4</v>
@@ -19730,7 +19730,7 @@
       </c>
       <c r="BA37">
         <f t="shared" si="30"/>
-        <v>19.198739823302532</v>
+        <v>9.2760308462576919</v>
       </c>
       <c r="BB37">
         <f t="shared" si="31"/>
@@ -19738,7 +19738,7 @@
       </c>
       <c r="BC37">
         <f t="shared" si="32"/>
-        <v>0.11575957879452443</v>
+        <v>5.6921416073739163E-2</v>
       </c>
       <c r="BD37">
         <f t="shared" si="33"/>
@@ -19821,10 +19821,10 @@
         <v>415.02800000000002</v>
       </c>
       <c r="BZ37">
-        <v>438.746732235519</v>
+        <v>427.33014644710403</v>
       </c>
       <c r="CA37">
-        <v>36.054656141389898</v>
+        <v>37.184611228278001</v>
       </c>
       <c r="CB37">
         <v>34.462200000000003</v>
@@ -20340,22 +20340,22 @@
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>6.4850178870513409</v>
+        <v>5.3204083211655755</v>
       </c>
       <c r="K38">
         <v>1629744252</v>
       </c>
       <c r="L38">
         <f t="shared" si="1"/>
-        <v>3.1346321060999639E-3</v>
+        <v>3.9543702838825672E-3</v>
       </c>
       <c r="M38">
         <f t="shared" si="2"/>
-        <v>3.1346321060999638</v>
+        <v>3.9543702838825672</v>
       </c>
       <c r="N38">
         <f t="shared" si="3"/>
-        <v>36.984548643731635</v>
+        <v>29.61453540484068</v>
       </c>
       <c r="O38">
         <f t="shared" si="4"/>
@@ -20363,11 +20363,11 @@
       </c>
       <c r="P38">
         <f t="shared" si="5"/>
-        <v>120.20741873175565</v>
+        <v>236.65344243237857</v>
       </c>
       <c r="Q38">
         <f t="shared" si="6"/>
-        <v>11.928779615664693</v>
+        <v>23.484297307504502</v>
       </c>
       <c r="R38">
         <f t="shared" si="7"/>
@@ -20375,7 +20375,7 @@
       </c>
       <c r="S38">
         <f t="shared" si="8"/>
-        <v>0.21225240153001557</v>
+        <v>0.29002834838466035</v>
       </c>
       <c r="T38">
         <f t="shared" si="9"/>
@@ -20383,11 +20383,11 @@
       </c>
       <c r="U38">
         <f t="shared" si="10"/>
-        <v>0.20403120553548301</v>
+        <v>0.2749089017566172</v>
       </c>
       <c r="V38">
         <f t="shared" si="11"/>
-        <v>0.12823161310707382</v>
+        <v>0.17311077648968026</v>
       </c>
       <c r="W38">
         <f t="shared" si="12"/>
@@ -20395,7 +20395,7 @@
       </c>
       <c r="X38">
         <f t="shared" si="13"/>
-        <v>34.658435981771781</v>
+        <v>34.44540270301939</v>
       </c>
       <c r="Y38">
         <f t="shared" si="14"/>
@@ -20407,11 +20407,11 @@
       </c>
       <c r="AA38">
         <f t="shared" si="16"/>
-        <v>72.797734727562101</v>
+        <v>74.587671658883366</v>
       </c>
       <c r="AB38">
         <f t="shared" si="17"/>
-        <v>3.7990490498141876</v>
+        <v>3.8924593492364412</v>
       </c>
       <c r="AC38">
         <f t="shared" si="18"/>
@@ -20419,11 +20419,11 @@
       </c>
       <c r="AD38">
         <f t="shared" si="19"/>
-        <v>1.455051817499462</v>
+        <v>1.3616415180772083</v>
       </c>
       <c r="AE38">
         <f t="shared" si="20"/>
-        <v>-138.23727587900842</v>
+        <v>-174.38772951922121</v>
       </c>
       <c r="AF38">
         <f t="shared" si="21"/>
@@ -20435,7 +20435,7 @@
       </c>
       <c r="AH38">
         <f t="shared" si="23"/>
-        <v>162.72472123319045</v>
+        <v>126.57426759297766</v>
       </c>
       <c r="AI38">
         <v>3</v>
@@ -20499,7 +20499,7 @@
       </c>
       <c r="BA38">
         <f t="shared" si="30"/>
-        <v>36.984548643731635</v>
+        <v>29.61453540484068</v>
       </c>
       <c r="BB38">
         <f t="shared" si="31"/>
@@ -20507,7 +20507,7 @@
       </c>
       <c r="BC38">
         <f t="shared" si="32"/>
-        <v>2.2191101108553976E-2</v>
+        <v>1.7807354939964614E-2</v>
       </c>
       <c r="BD38">
         <f t="shared" si="33"/>
@@ -20590,10 +20590,10 @@
         <v>415.17099999999999</v>
       </c>
       <c r="BZ38">
-        <v>461.10165524959598</v>
+        <v>452.668331049919</v>
       </c>
       <c r="CA38">
-        <v>38.283369684673801</v>
+        <v>39.224673936934799</v>
       </c>
       <c r="CB38">
         <v>34.666800000000002</v>
@@ -21109,22 +21109,22 @@
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>6.7748506044301031</v>
+        <v>4.6405423757174136</v>
       </c>
       <c r="K39">
         <v>1629744755.5</v>
       </c>
       <c r="L39">
         <f t="shared" si="1"/>
-        <v>4.4893759003995616E-3</v>
+        <v>3.1557515215618641E-3</v>
       </c>
       <c r="M39">
         <f t="shared" si="2"/>
-        <v>4.4893759003995619</v>
+        <v>3.1557515215618639</v>
       </c>
       <c r="N39">
         <f t="shared" si="3"/>
-        <v>35.802955106093208</v>
+        <v>25.492278308493084</v>
       </c>
       <c r="O39">
         <f t="shared" si="4"/>
@@ -21132,11 +21132,11 @@
       </c>
       <c r="P39">
         <f t="shared" si="5"/>
-        <v>268.93430647736909</v>
+        <v>245.42452334266974</v>
       </c>
       <c r="Q39">
         <f t="shared" si="6"/>
-        <v>26.68968787279637</v>
+        <v>24.356520408811779</v>
       </c>
       <c r="R39">
         <f t="shared" si="7"/>
@@ -21144,7 +21144,7 @@
       </c>
       <c r="S39">
         <f t="shared" si="8"/>
-        <v>0.43801442606935626</v>
+        <v>0.26095998861785569</v>
       </c>
       <c r="T39">
         <f t="shared" si="9"/>
@@ -21152,11 +21152,11 @@
       </c>
       <c r="U39">
         <f t="shared" si="10"/>
-        <v>0.40450440503628665</v>
+        <v>0.24865732425614448</v>
       </c>
       <c r="V39">
         <f t="shared" si="11"/>
-        <v>0.25561202198457506</v>
+        <v>0.15646783107486159</v>
       </c>
       <c r="W39">
         <f t="shared" si="12"/>
@@ -21164,7 +21164,7 @@
       </c>
       <c r="X39">
         <f t="shared" si="13"/>
-        <v>33.010727193280914</v>
+        <v>33.357226868601025</v>
       </c>
       <c r="Y39">
         <f t="shared" si="14"/>
@@ -21176,11 +21176,11 @@
       </c>
       <c r="AA39">
         <f t="shared" si="16"/>
-        <v>78.530311012367434</v>
+        <v>75.546884705872145</v>
       </c>
       <c r="AB39">
         <f t="shared" si="17"/>
-        <v>3.9963729438621964</v>
+        <v>3.8445476929803193</v>
       </c>
       <c r="AC39">
         <f t="shared" si="18"/>
@@ -21188,11 +21188,11 @@
       </c>
       <c r="AD39">
         <f t="shared" si="19"/>
-        <v>1.0512506526118539</v>
+        <v>1.2030759034937311</v>
       </c>
       <c r="AE39">
         <f t="shared" si="20"/>
-        <v>-197.98147720762066</v>
+        <v>-139.1686421008782</v>
       </c>
       <c r="AF39">
         <f t="shared" si="21"/>
@@ -21204,7 +21204,7 @@
       </c>
       <c r="AH39">
         <f t="shared" si="23"/>
-        <v>4.5012944429799013</v>
+        <v>63.314129549722352</v>
       </c>
       <c r="AI39">
         <v>2</v>
@@ -21268,7 +21268,7 @@
       </c>
       <c r="BA39">
         <f t="shared" si="30"/>
-        <v>35.802955106093208</v>
+        <v>25.492278308493084</v>
       </c>
       <c r="BB39">
         <f t="shared" si="31"/>
@@ -21276,7 +21276,7 @@
       </c>
       <c r="BC39">
         <f t="shared" si="32"/>
-        <v>3.9048565072271543E-2</v>
+        <v>2.7903881446436414E-2</v>
       </c>
       <c r="BD39">
         <f t="shared" si="33"/>
@@ -21359,10 +21359,10 @@
         <v>415.00799999999998</v>
       </c>
       <c r="BZ39">
-        <v>460.19934474704399</v>
+        <v>447.16466894940902</v>
       </c>
       <c r="CA39">
-        <v>40.268803112454499</v>
+        <v>38.7389606224909</v>
       </c>
       <c r="CB39">
         <v>35.099400000000003</v>
@@ -21878,22 +21878,22 @@
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>5.7407471787565214</v>
+        <v>4.0614733695096206</v>
       </c>
       <c r="K40">
         <v>1629745065.0999999</v>
       </c>
       <c r="L40">
         <f t="shared" si="1"/>
-        <v>3.5221579845754456E-3</v>
+        <v>2.797773228176168E-3</v>
       </c>
       <c r="M40">
         <f t="shared" si="2"/>
-        <v>3.5221579845754456</v>
+        <v>2.797773228176168</v>
       </c>
       <c r="N40">
         <f t="shared" si="3"/>
-        <v>30.733549934840454</v>
+        <v>22.218165140545299</v>
       </c>
       <c r="O40">
         <f t="shared" si="4"/>
@@ -21901,11 +21901,11 @@
       </c>
       <c r="P40">
         <f t="shared" si="5"/>
-        <v>257.12270429993686</v>
+        <v>259.04873752699643</v>
       </c>
       <c r="Q40">
         <f t="shared" si="6"/>
-        <v>25.51542731536712</v>
+        <v>25.706556142149736</v>
       </c>
       <c r="R40">
         <f t="shared" si="7"/>
@@ -21913,7 +21913,7 @@
       </c>
       <c r="S40">
         <f t="shared" si="8"/>
-        <v>0.34138354208704447</v>
+        <v>0.24715975625692274</v>
       </c>
       <c r="T40">
         <f t="shared" si="9"/>
@@ -21921,11 +21921,11 @@
       </c>
       <c r="U40">
         <f t="shared" si="10"/>
-        <v>0.3206185356871421</v>
+        <v>0.23607556937907728</v>
       </c>
       <c r="V40">
         <f t="shared" si="11"/>
-        <v>0.20214689874583003</v>
+        <v>0.1485016734744789</v>
       </c>
       <c r="W40">
         <f t="shared" si="12"/>
@@ -21933,7 +21933,7 @@
       </c>
       <c r="X40">
         <f t="shared" si="13"/>
-        <v>32.617833793291794</v>
+        <v>32.80639992221225</v>
       </c>
       <c r="Y40">
         <f t="shared" si="14"/>
@@ -21945,11 +21945,11 @@
       </c>
       <c r="AA40">
         <f t="shared" si="16"/>
-        <v>77.520834875752442</v>
+        <v>75.864424371287072</v>
       </c>
       <c r="AB40">
         <f t="shared" si="17"/>
-        <v>3.865540305057062</v>
+        <v>3.7829441671672521</v>
       </c>
       <c r="AC40">
         <f t="shared" si="18"/>
@@ -21957,11 +21957,11 @@
       </c>
       <c r="AD40">
         <f t="shared" si="19"/>
-        <v>1.0419527560778907</v>
+        <v>1.1245488939677006</v>
       </c>
       <c r="AE40">
         <f t="shared" si="20"/>
-        <v>-155.32716711977716</v>
+        <v>-123.38179936256901</v>
       </c>
       <c r="AF40">
         <f t="shared" si="21"/>
@@ -21973,7 +21973,7 @@
       </c>
       <c r="AH40">
         <f t="shared" si="23"/>
-        <v>22.651264074502983</v>
+        <v>54.596631831711129</v>
       </c>
       <c r="AI40">
         <v>3</v>
@@ -22037,7 +22037,7 @@
       </c>
       <c r="BA40">
         <f t="shared" si="30"/>
-        <v>30.733549934840454</v>
+        <v>22.218165140545299</v>
       </c>
       <c r="BB40">
         <f t="shared" si="31"/>
@@ -22045,7 +22045,7 @@
       </c>
       <c r="BC40">
         <f t="shared" si="32"/>
-        <v>4.6131229664113295E-2</v>
+        <v>3.3482698771781637E-2</v>
       </c>
       <c r="BD40">
         <f t="shared" si="33"/>
@@ -22128,10 +22128,10 @@
         <v>415.01400000000001</v>
       </c>
       <c r="BZ40">
-        <v>453.63568585742001</v>
+        <v>443.05993717148402</v>
       </c>
       <c r="CA40">
-        <v>38.953616748486503</v>
+        <v>38.1212833496973</v>
       </c>
       <c r="CB40">
         <v>34.893000000000001</v>
@@ -22647,22 +22647,22 @@
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
-        <v>1.8998207761226629</v>
+        <v>2.9640471375988304</v>
       </c>
       <c r="K41">
         <v>1629745473.0999999</v>
       </c>
       <c r="L41">
         <f t="shared" si="1"/>
-        <v>3.4237687440226076E-3</v>
+        <v>2.5578693299642325E-3</v>
       </c>
       <c r="M41">
         <f t="shared" si="2"/>
-        <v>3.4237687440226074</v>
+        <v>2.5578693299642326</v>
       </c>
       <c r="N41">
         <f t="shared" si="3"/>
-        <v>10.205472283500502</v>
+        <v>16.345888123634566</v>
       </c>
       <c r="O41">
         <f t="shared" si="4"/>
@@ -22670,11 +22670,11 @@
       </c>
       <c r="P41">
         <f t="shared" si="5"/>
-        <v>356.93058224275234</v>
+        <v>287.30538737750317</v>
       </c>
       <c r="Q41">
         <f t="shared" si="6"/>
-        <v>35.421369803683696</v>
+        <v>28.511847622986309</v>
       </c>
       <c r="R41">
         <f t="shared" si="7"/>
@@ -22682,7 +22682,7 @@
       </c>
       <c r="S41">
         <f t="shared" si="8"/>
-        <v>0.33491732365381216</v>
+        <v>0.22395229729926439</v>
       </c>
       <c r="T41">
         <f t="shared" si="9"/>
@@ -22690,11 +22690,11 @@
       </c>
       <c r="U41">
         <f t="shared" si="10"/>
-        <v>0.31489036714504592</v>
+        <v>0.21480288609855114</v>
       </c>
       <c r="V41">
         <f t="shared" si="11"/>
-        <v>0.19850595068429225</v>
+        <v>0.13504269474307787</v>
       </c>
       <c r="W41">
         <f t="shared" si="12"/>
@@ -22702,7 +22702,7 @@
       </c>
       <c r="X41">
         <f t="shared" si="13"/>
-        <v>32.322827381045101</v>
+        <v>32.548443250277991</v>
       </c>
       <c r="Y41">
         <f t="shared" si="14"/>
@@ -22714,11 +22714,11 @@
       </c>
       <c r="AA41">
         <f t="shared" si="16"/>
-        <v>77.254996179333872</v>
+        <v>75.252968131955214</v>
       </c>
       <c r="AB41">
         <f t="shared" si="17"/>
-        <v>3.8136216961170848</v>
+        <v>3.714793426421815</v>
       </c>
       <c r="AC41">
         <f t="shared" si="18"/>
@@ -22726,11 +22726,11 @@
       </c>
       <c r="AD41">
         <f t="shared" si="19"/>
-        <v>1.0319377382172257</v>
+        <v>1.1307660079124955</v>
       </c>
       <c r="AE41">
         <f t="shared" si="20"/>
-        <v>-150.98820161139699</v>
+        <v>-112.80203745142265</v>
       </c>
       <c r="AF41">
         <f t="shared" si="21"/>
@@ -22742,7 +22742,7 @@
       </c>
       <c r="AH41">
         <f t="shared" si="23"/>
-        <v>10.779513973662532</v>
+        <v>48.965678133636871</v>
       </c>
       <c r="AI41">
         <v>2</v>
@@ -22806,7 +22806,7 @@
       </c>
       <c r="BA41">
         <f t="shared" si="30"/>
-        <v>10.205472283500502</v>
+        <v>16.345888123634566</v>
       </c>
       <c r="BB41">
         <f t="shared" si="31"/>
@@ -22814,7 +22814,7 @@
       </c>
       <c r="BC41">
         <f t="shared" si="32"/>
-        <v>1.9241385613519128E-2</v>
+        <v>3.0462888529895212E-2</v>
       </c>
       <c r="BD41">
         <f t="shared" si="33"/>
@@ -22897,10 +22897,10 @@
         <v>414.99900000000002</v>
       </c>
       <c r="BZ41">
-        <v>428.94739133619402</v>
+        <v>435.883078267239</v>
       </c>
       <c r="CA41">
-        <v>38.428728758736597</v>
+        <v>37.4328657517473</v>
       </c>
       <c r="CB41">
         <v>34.478999999999999</v>
@@ -23416,22 +23416,22 @@
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>0.28366288153377317</v>
+        <v>2.2074687155699286</v>
       </c>
       <c r="K42">
         <v>1629745788.0999999</v>
       </c>
       <c r="L42">
         <f t="shared" si="1"/>
-        <v>3.6088302916355247E-3</v>
+        <v>2.5373596140149837E-3</v>
       </c>
       <c r="M42">
         <f t="shared" si="2"/>
-        <v>3.6088302916355248</v>
+        <v>2.5373596140149837</v>
       </c>
       <c r="N42">
         <f t="shared" si="3"/>
-        <v>1.506525500000238</v>
+        <v>12.106346685641157</v>
       </c>
       <c r="O42">
         <f t="shared" si="4"/>
@@ -23439,11 +23439,11 @@
       </c>
       <c r="P42">
         <f t="shared" si="5"/>
-        <v>401.19560305830976</v>
+        <v>318.2789927299699</v>
       </c>
       <c r="Q42">
         <f t="shared" si="6"/>
-        <v>39.814000145966851</v>
+        <v>31.585490385265921</v>
       </c>
       <c r="R42">
         <f t="shared" si="7"/>
@@ -23451,7 +23451,7 @@
       </c>
       <c r="S42">
         <f t="shared" si="8"/>
-        <v>0.36561063915502195</v>
+        <v>0.22348129821335663</v>
       </c>
       <c r="T42">
         <f t="shared" si="9"/>
@@ -23459,11 +23459,11 @@
       </c>
       <c r="U42">
         <f t="shared" si="10"/>
-        <v>0.34191407235239507</v>
+        <v>0.2143812577010944</v>
       </c>
       <c r="V42">
         <f t="shared" si="11"/>
-        <v>0.21569722156168297</v>
+        <v>0.13477501169494699</v>
       </c>
       <c r="W42">
         <f t="shared" si="12"/>
@@ -23471,7 +23471,7 @@
       </c>
       <c r="X42">
         <f t="shared" si="13"/>
-        <v>32.185650148856666</v>
+        <v>32.464468930962695</v>
       </c>
       <c r="Y42">
         <f t="shared" si="14"/>
@@ -23483,11 +23483,11 @@
       </c>
       <c r="AA42">
         <f t="shared" si="16"/>
-        <v>78.141634601969585</v>
+        <v>75.672471679488083</v>
       </c>
       <c r="AB42">
         <f t="shared" si="17"/>
-        <v>3.8687086162191417</v>
+        <v>3.7464630051347241</v>
       </c>
       <c r="AC42">
         <f t="shared" si="18"/>
@@ -23495,11 +23495,11 @@
       </c>
       <c r="AD42">
         <f t="shared" si="19"/>
-        <v>1.001322179158215</v>
+        <v>1.1235677902426326</v>
       </c>
       <c r="AE42">
         <f t="shared" si="20"/>
-        <v>-159.14941586112664</v>
+        <v>-111.89755897806079</v>
       </c>
       <c r="AF42">
         <f t="shared" si="21"/>
@@ -23511,7 +23511,7 @@
       </c>
       <c r="AH42">
         <f t="shared" si="23"/>
-        <v>-27.569670863831121</v>
+        <v>19.682186019234734</v>
       </c>
       <c r="AI42">
         <v>2</v>
@@ -23575,7 +23575,7 @@
       </c>
       <c r="BA42">
         <f t="shared" si="30"/>
-        <v>1.506525500000238</v>
+        <v>12.106346685641157</v>
       </c>
       <c r="BB42">
         <f t="shared" si="31"/>
@@ -23583,7 +23583,7 @@
       </c>
       <c r="BC42">
         <f t="shared" si="32"/>
-        <v>4.3444326015040684E-3</v>
+        <v>2.950909138884257E-2</v>
       </c>
       <c r="BD42">
         <f t="shared" si="33"/>
@@ -23666,10 +23666,10 @@
         <v>415.00799999999998</v>
       </c>
       <c r="BZ42">
-        <v>418.61291132372997</v>
+        <v>430.79858226474602</v>
       </c>
       <c r="CA42">
-        <v>38.983997605127499</v>
+        <v>37.752159521025497</v>
       </c>
       <c r="CB42">
         <v>34.822400000000002</v>
@@ -24185,22 +24185,22 @@
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
-        <v>3.4769651064281231</v>
+        <v>2.2044699149011278</v>
       </c>
       <c r="K43">
         <v>1629746202.5999999</v>
       </c>
       <c r="L43">
         <f t="shared" si="1"/>
-        <v>3.4297473196409061E-3</v>
+        <v>2.1976045608684096E-3</v>
       </c>
       <c r="M43">
         <f t="shared" si="2"/>
-        <v>3.4297473196409061</v>
+        <v>2.1976045608684096</v>
       </c>
       <c r="N43">
         <f t="shared" si="3"/>
-        <v>18.298671201827894</v>
+        <v>12.044691604838992</v>
       </c>
       <c r="O43">
         <f t="shared" si="4"/>
@@ -24208,11 +24208,11 @@
       </c>
       <c r="P43">
         <f t="shared" si="5"/>
-        <v>328.14510511710188</v>
+        <v>311.9638579490084</v>
       </c>
       <c r="Q43">
         <f t="shared" si="6"/>
-        <v>32.564881342184663</v>
+        <v>30.959066153171008</v>
       </c>
       <c r="R43">
         <f t="shared" si="7"/>
@@ -24220,7 +24220,7 @@
       </c>
       <c r="S43">
         <f t="shared" si="8"/>
-        <v>0.38291819141725203</v>
+        <v>0.206087285363204</v>
       </c>
       <c r="T43">
         <f t="shared" si="9"/>
@@ -24228,11 +24228,11 @@
       </c>
       <c r="U43">
         <f t="shared" si="10"/>
-        <v>0.35693419197828613</v>
+        <v>0.19829862077913049</v>
       </c>
       <c r="V43">
         <f t="shared" si="11"/>
-        <v>0.22527132624953999</v>
+        <v>0.12461189321784244</v>
       </c>
       <c r="W43">
         <f t="shared" si="12"/>
@@ -24240,7 +24240,7 @@
       </c>
       <c r="X43">
         <f t="shared" si="13"/>
-        <v>31.726717649317912</v>
+        <v>32.048370478679779</v>
       </c>
       <c r="Y43">
         <f t="shared" si="14"/>
@@ -24252,11 +24252,11 @@
       </c>
       <c r="AA43">
         <f t="shared" si="16"/>
-        <v>78.861014886530512</v>
+        <v>75.960895283833636</v>
       </c>
       <c r="AB43">
         <f t="shared" si="17"/>
-        <v>3.8256634133020073</v>
+        <v>3.6849743608696834</v>
       </c>
       <c r="AC43">
         <f t="shared" si="18"/>
@@ -24264,11 +24264,11 @@
       </c>
       <c r="AD43">
         <f t="shared" si="19"/>
-        <v>0.91243669553484619</v>
+        <v>1.0531257479671701</v>
       </c>
       <c r="AE43">
         <f t="shared" si="20"/>
-        <v>-151.25185679616396</v>
+        <v>-96.914361134296868</v>
       </c>
       <c r="AF43">
         <f t="shared" si="21"/>
@@ -24280,7 +24280,7 @@
       </c>
       <c r="AH43">
         <f t="shared" si="23"/>
-        <v>-22.982242793340944</v>
+        <v>31.355252868526151</v>
       </c>
       <c r="AI43">
         <v>3</v>
@@ -24344,7 +24344,7 @@
       </c>
       <c r="BA43">
         <f t="shared" si="30"/>
-        <v>18.298671201827894</v>
+        <v>12.044691604838992</v>
       </c>
       <c r="BB43">
         <f t="shared" si="31"/>
@@ -24352,7 +24352,7 @@
       </c>
       <c r="BC43">
         <f t="shared" si="32"/>
-        <v>6.310516731769146E-2</v>
+        <v>4.1912154666423451E-2</v>
       </c>
       <c r="BD43">
         <f t="shared" si="33"/>
@@ -24435,10 +24435,10 @@
         <v>415.03199999999998</v>
       </c>
       <c r="BZ43">
-        <v>438.69590095276499</v>
+        <v>430.57838019055299</v>
       </c>
       <c r="CA43">
-        <v>38.549893970423398</v>
+        <v>37.1322187940847</v>
       </c>
       <c r="CB43">
         <v>34.593299999999999</v>
@@ -24954,22 +24954,22 @@
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
-        <v>3.0247968763093049</v>
+        <v>1.4105255102625769</v>
       </c>
       <c r="K44">
         <v>1629746858</v>
       </c>
       <c r="L44">
         <f t="shared" si="1"/>
-        <v>1.1857929372768043E-4</v>
+        <v>9.7429135701734707E-4</v>
       </c>
       <c r="M44">
         <f t="shared" si="2"/>
-        <v>0.11857929372768043</v>
+        <v>0.97429135701734704</v>
       </c>
       <c r="N44">
         <f t="shared" si="3"/>
-        <v>17.305965803199683</v>
+        <v>7.849870234429944</v>
       </c>
       <c r="O44">
         <f t="shared" si="4"/>
@@ -24977,11 +24977,11 @@
       </c>
       <c r="P44">
         <f t="shared" si="5"/>
-        <v>-2585.185367793657</v>
+        <v>255.26999802405888</v>
       </c>
       <c r="Q44">
         <f t="shared" si="6"/>
-        <v>-256.49325577038104</v>
+        <v>25.327016665566877</v>
       </c>
       <c r="R44">
         <f t="shared" si="7"/>
@@ -24989,7 +24989,7 @@
       </c>
       <c r="S44">
         <f t="shared" si="8"/>
-        <v>9.1744181181232318E-3</v>
+        <v>8.3017451773793063E-2</v>
       </c>
       <c r="T44">
         <f t="shared" si="9"/>
@@ -24997,11 +24997,11 @@
       </c>
       <c r="U44">
         <f t="shared" si="10"/>
-        <v>9.1583953619581958E-3</v>
+        <v>8.1725098321033571E-2</v>
       </c>
       <c r="V44">
         <f t="shared" si="11"/>
-        <v>5.725434320574159E-3</v>
+        <v>5.1192623376824328E-2</v>
       </c>
       <c r="W44">
         <f t="shared" si="12"/>
@@ -25009,7 +25009,7 @@
       </c>
       <c r="X44">
         <f t="shared" si="13"/>
-        <v>32.342058733468477</v>
+        <v>32.119144180169698</v>
       </c>
       <c r="Y44">
         <f t="shared" si="14"/>
@@ -25021,11 +25021,11 @@
       </c>
       <c r="AA44">
         <f t="shared" si="16"/>
-        <v>72.533045562459336</v>
+        <v>74.568259470770002</v>
       </c>
       <c r="AB44">
         <f t="shared" si="17"/>
-        <v>3.4984623713144245</v>
+        <v>3.5966261699056394</v>
       </c>
       <c r="AC44">
         <f t="shared" si="18"/>
@@ -25033,11 +25033,11 @@
       </c>
       <c r="AD44">
         <f t="shared" si="19"/>
-        <v>1.2313489775133597</v>
+        <v>1.1331851789221448</v>
       </c>
       <c r="AE44">
         <f t="shared" si="20"/>
-        <v>-5.229346853390707</v>
+        <v>-42.966248844465007</v>
       </c>
       <c r="AF44">
         <f t="shared" si="21"/>
@@ -25049,7 +25049,7 @@
       </c>
       <c r="AH44">
         <f t="shared" si="23"/>
-        <v>86.373819093644855</v>
+        <v>48.636917102570557</v>
       </c>
       <c r="AI44">
         <v>2</v>
@@ -25113,7 +25113,7 @@
       </c>
       <c r="BA44">
         <f t="shared" si="30"/>
-        <v>17.305965803199683</v>
+        <v>7.849870234429944</v>
       </c>
       <c r="BB44">
         <f t="shared" si="31"/>
@@ -25121,7 +25121,7 @@
       </c>
       <c r="BC44">
         <f t="shared" si="32"/>
-        <v>0.10444974183679143</v>
+        <v>4.8424751227736193E-2</v>
       </c>
       <c r="BD44">
         <f t="shared" si="33"/>
@@ -25204,10 +25204,10 @@
         <v>414.988</v>
       </c>
       <c r="BZ44">
-        <v>435.81208568783399</v>
+        <v>424.892017137567</v>
       </c>
       <c r="CA44">
-        <v>35.2608637015989</v>
+        <v>36.250252740319802</v>
       </c>
       <c r="CB44">
         <v>35.123600000000003</v>

</xml_diff>